<commit_message>
update hasil testing, buku TA
</commit_message>
<xml_diff>
--- a/Data Hasil Uji Coba/Uji Coba.xlsx
+++ b/Data Hasil Uji Coba/Uji Coba.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="121">
   <si>
     <t>0 x</t>
   </si>
@@ -362,25 +362,49 @@
     <t>Rata - rata</t>
   </si>
   <si>
-    <t>Panjang Data 584</t>
-  </si>
-  <si>
     <t>Efektifitas</t>
   </si>
   <si>
     <t>Waktu</t>
   </si>
   <si>
-    <t>Panjang Data 980</t>
+    <t>FAIL</t>
   </si>
   <si>
-    <t>Panjang Data 1280</t>
+    <t>Uji Coba</t>
   </si>
   <si>
-    <t>Panjang Data 1345</t>
+    <t>Konfigurasi</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Efektifitas Kompresi Pada Panjang Data 584</t>
+  </si>
+  <si>
+    <t>Efektifitas Kompresi Pada Panjang Data 980</t>
+  </si>
+  <si>
+    <t>Efektifitas Kompresi Pada Panjang Data 1280</t>
+  </si>
+  <si>
+    <t>Efektifitas Kompresi Pada Panjang Data 1345</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Rata -rata</t>
+  </si>
+  <si>
+    <t>Waktu Kompresi Pada Panjang Data 584</t>
+  </si>
+  <si>
+    <t>Waktu Kompresi Pada Panjang Data 980</t>
+  </si>
+  <si>
+    <t>Waktu Kompresi Pada Panjang Data 1280</t>
+  </si>
+  <si>
+    <t>Waktu Kompresi Pada Panjang Data 1345</t>
   </si>
 </sst>
 </file>
@@ -690,7 +714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -806,32 +830,35 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -869,25 +896,31 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -909,18 +942,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -950,29 +992,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2366,32 +2402,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="K2" s="59" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="K2" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="61"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
         <v>1</v>
@@ -2408,10 +2444,10 @@
       <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="60" t="s">
+      <c r="K3" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="61"/>
+      <c r="L3" s="82"/>
       <c r="M3" s="14"/>
       <c r="N3" s="15" t="s">
         <v>1</v>
@@ -2430,10 +2466,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="62">
+      <c r="A4" s="63">
         <v>584</v>
       </c>
-      <c r="B4" s="63"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -2452,10 +2488,10 @@
       <c r="H4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="62">
+      <c r="K4" s="63">
         <v>584</v>
       </c>
-      <c r="L4" s="63"/>
+      <c r="L4" s="64"/>
       <c r="M4" s="1" t="s">
         <v>30</v>
       </c>
@@ -2476,8 +2512,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="65"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -2496,8 +2532,8 @@
       <c r="H5" s="1">
         <v>21</v>
       </c>
-      <c r="K5" s="64"/>
-      <c r="L5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="66"/>
       <c r="M5" s="1" t="s">
         <v>21</v>
       </c>
@@ -2518,8 +2554,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2543,8 +2579,8 @@
         <f>($A$4-H5)/$A$4</f>
         <v>0.96404109589041098</v>
       </c>
-      <c r="K6" s="64"/>
-      <c r="L6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="66"/>
       <c r="M6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2570,8 +2606,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
-      <c r="B7" s="65"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2590,8 +2626,8 @@
       <c r="H7" s="1">
         <v>427</v>
       </c>
-      <c r="K7" s="64"/>
-      <c r="L7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="66"/>
       <c r="M7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2612,8 +2648,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
@@ -2637,8 +2673,8 @@
         <f>($A$4-H7)/$A$4</f>
         <v>0.26883561643835618</v>
       </c>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="68"/>
       <c r="M8" s="1" t="s">
         <v>34</v>
       </c>
@@ -2664,10 +2700,10 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="68">
+      <c r="A9" s="69">
         <v>980</v>
       </c>
-      <c r="B9" s="69"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="16" t="s">
         <v>30</v>
       </c>
@@ -2686,10 +2722,10 @@
       <c r="H9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="68">
+      <c r="K9" s="69">
         <v>980</v>
       </c>
-      <c r="L9" s="69"/>
+      <c r="L9" s="70"/>
       <c r="M9" s="16" t="s">
         <v>30</v>
       </c>
@@ -2710,8 +2746,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="16" t="s">
         <v>21</v>
       </c>
@@ -2730,8 +2766,8 @@
       <c r="H10" s="16">
         <v>33</v>
       </c>
-      <c r="K10" s="70"/>
-      <c r="L10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="72"/>
       <c r="M10" s="16" t="s">
         <v>21</v>
       </c>
@@ -2752,8 +2788,8 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="71"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
@@ -2777,8 +2813,8 @@
         <f>($A$9-H10)/$A$9</f>
         <v>0.96632653061224494</v>
       </c>
-      <c r="K11" s="70"/>
-      <c r="L11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="72"/>
       <c r="M11" s="16" t="s">
         <v>35</v>
       </c>
@@ -2804,8 +2840,8 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="70"/>
-      <c r="B12" s="71"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="16" t="s">
         <v>22</v>
       </c>
@@ -2824,8 +2860,8 @@
       <c r="H12" s="16">
         <v>564</v>
       </c>
-      <c r="K12" s="70"/>
-      <c r="L12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="72"/>
       <c r="M12" s="16" t="s">
         <v>22</v>
       </c>
@@ -2846,8 +2882,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
-      <c r="B13" s="73"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="16" t="s">
         <v>34</v>
       </c>
@@ -2871,8 +2907,8 @@
         <f>($A$9-H12)/$A$9</f>
         <v>0.42448979591836733</v>
       </c>
-      <c r="K13" s="72"/>
-      <c r="L13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="74"/>
       <c r="M13" s="16" t="s">
         <v>34</v>
       </c>
@@ -2898,10 +2934,10 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="53">
+      <c r="A14" s="75">
         <v>1280</v>
       </c>
-      <c r="B14" s="54"/>
+      <c r="B14" s="76"/>
       <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
@@ -2920,10 +2956,10 @@
       <c r="H14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="53">
+      <c r="K14" s="75">
         <v>1280</v>
       </c>
-      <c r="L14" s="54"/>
+      <c r="L14" s="76"/>
       <c r="M14" s="13" t="s">
         <v>30</v>
       </c>
@@ -2944,8 +2980,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="56"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
@@ -2962,8 +2998,8 @@
         <v>68</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="56"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="78"/>
       <c r="M15" s="4" t="s">
         <v>21</v>
       </c>
@@ -2984,8 +3020,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
@@ -3009,8 +3045,8 @@
         <f>($A$14-H15)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K16" s="55"/>
-      <c r="L16" s="56"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="78"/>
       <c r="M16" s="4" t="s">
         <v>35</v>
       </c>
@@ -3036,8 +3072,8 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="56"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3054,8 +3090,8 @@
         <v>1120</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="56"/>
+      <c r="K17" s="77"/>
+      <c r="L17" s="78"/>
       <c r="M17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3076,8 +3112,8 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="58"/>
+      <c r="A18" s="79"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
@@ -3101,8 +3137,8 @@
         <f>($A$14-H17)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K18" s="57"/>
-      <c r="L18" s="58"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="80"/>
       <c r="M18" s="4" t="s">
         <v>34</v>
       </c>
@@ -3128,10 +3164,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="74">
+      <c r="A19" s="56">
         <v>1345</v>
       </c>
-      <c r="B19" s="75"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
@@ -3150,10 +3186,10 @@
       <c r="H19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K19" s="74">
+      <c r="K19" s="56">
         <v>1345</v>
       </c>
-      <c r="L19" s="75"/>
+      <c r="L19" s="57"/>
       <c r="M19" s="7" t="s">
         <v>30</v>
       </c>
@@ -3174,8 +3210,8 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="76"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
@@ -3192,8 +3228,8 @@
         <v>129</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="77"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="59"/>
       <c r="M20" s="7" t="s">
         <v>21</v>
       </c>
@@ -3214,8 +3250,8 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="7" t="s">
         <v>35</v>
       </c>
@@ -3236,8 +3272,8 @@
         <v>0.90408921933085507</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="77"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="59"/>
       <c r="M21" s="7" t="s">
         <v>35</v>
       </c>
@@ -3263,8 +3299,8 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="76"/>
-      <c r="B22" s="77"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
@@ -3281,8 +3317,8 @@
         <v>1182</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="77"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="59"/>
       <c r="M22" s="7" t="s">
         <v>22</v>
       </c>
@@ -3301,8 +3337,8 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="78"/>
-      <c r="B23" s="79"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="7" t="s">
         <v>34</v>
       </c>
@@ -3323,8 +3359,8 @@
         <v>0.12118959107806691</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="79"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="61"/>
       <c r="M23" s="7" t="s">
         <v>34</v>
       </c>
@@ -3347,10 +3383,10 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K24" s="80">
+      <c r="K24" s="62">
         <v>1640</v>
       </c>
-      <c r="L24" s="80"/>
+      <c r="L24" s="62"/>
       <c r="M24" s="24" t="s">
         <v>30</v>
       </c>
@@ -3371,10 +3407,10 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="61"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
         <v>1</v>
@@ -3391,10 +3427,10 @@
       <c r="H28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="60" t="s">
+      <c r="K28" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="L28" s="61"/>
+      <c r="L28" s="82"/>
       <c r="M28" s="14"/>
       <c r="N28" s="15" t="s">
         <v>1</v>
@@ -3413,10 +3449,10 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="62">
+      <c r="A29" s="63">
         <v>584</v>
       </c>
-      <c r="B29" s="63"/>
+      <c r="B29" s="64"/>
       <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
@@ -3436,10 +3472,10 @@
         <v>8.1119999999999994E-3</v>
       </c>
       <c r="J29" s="24"/>
-      <c r="K29" s="62">
+      <c r="K29" s="63">
         <v>584</v>
       </c>
-      <c r="L29" s="63"/>
+      <c r="L29" s="64"/>
       <c r="M29" s="1" t="s">
         <v>23</v>
       </c>
@@ -3460,8 +3496,8 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="64"/>
-      <c r="B30" s="65"/>
+      <c r="A30" s="65"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
@@ -3480,8 +3516,8 @@
       <c r="H30" s="1">
         <v>3.248E-3</v>
       </c>
-      <c r="K30" s="64"/>
-      <c r="L30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="66"/>
       <c r="M30" s="1" t="s">
         <v>24</v>
       </c>
@@ -3502,8 +3538,8 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
-      <c r="B31" s="65"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="66"/>
       <c r="C31" s="19" t="s">
         <v>32</v>
       </c>
@@ -3527,8 +3563,8 @@
         <f t="shared" si="0"/>
         <v>1.1359999999999999E-2</v>
       </c>
-      <c r="K31" s="64"/>
-      <c r="L31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="66"/>
       <c r="M31" s="19" t="s">
         <v>32</v>
       </c>
@@ -3554,8 +3590,8 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
-      <c r="B32" s="65"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3575,8 +3611,8 @@
         <v>4.0691999999999999E-2</v>
       </c>
       <c r="J32" s="24"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="66"/>
       <c r="M32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3597,8 +3633,8 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="64"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="66"/>
       <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3617,8 +3653,8 @@
       <c r="H33" s="1">
         <v>1.7328E-2</v>
       </c>
-      <c r="K33" s="64"/>
-      <c r="L33" s="65"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="66"/>
       <c r="M33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3639,8 +3675,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="66"/>
-      <c r="B34" s="67"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="68"/>
       <c r="C34" s="19" t="s">
         <v>32</v>
       </c>
@@ -3664,8 +3700,8 @@
         <f t="shared" si="2"/>
         <v>5.8020000000000002E-2</v>
       </c>
-      <c r="K34" s="66"/>
-      <c r="L34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="68"/>
       <c r="M34" s="19" t="s">
         <v>32</v>
       </c>
@@ -3691,10 +3727,10 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="68">
+      <c r="A35" s="69">
         <v>980</v>
       </c>
-      <c r="B35" s="69"/>
+      <c r="B35" s="70"/>
       <c r="C35" s="16" t="s">
         <v>23</v>
       </c>
@@ -3714,10 +3750,10 @@
         <v>1.2716E-2</v>
       </c>
       <c r="J35" s="24"/>
-      <c r="K35" s="68">
+      <c r="K35" s="69">
         <v>980</v>
       </c>
-      <c r="L35" s="69"/>
+      <c r="L35" s="70"/>
       <c r="M35" s="16" t="s">
         <v>23</v>
       </c>
@@ -3738,8 +3774,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" s="71"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="16" t="s">
         <v>24</v>
       </c>
@@ -3758,8 +3794,8 @@
       <c r="H36" s="16">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="K36" s="70"/>
-      <c r="L36" s="71"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="72"/>
       <c r="M36" s="16" t="s">
         <v>24</v>
       </c>
@@ -3780,8 +3816,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="70"/>
-      <c r="B37" s="71"/>
+      <c r="A37" s="71"/>
+      <c r="B37" s="72"/>
       <c r="C37" s="19" t="s">
         <v>32</v>
       </c>
@@ -3805,8 +3841,8 @@
         <f t="shared" si="4"/>
         <v>1.7916000000000001E-2</v>
       </c>
-      <c r="K37" s="70"/>
-      <c r="L37" s="71"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="72"/>
       <c r="M37" s="19" t="s">
         <v>32</v>
       </c>
@@ -3832,8 +3868,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="70"/>
-      <c r="B38" s="71"/>
+      <c r="A38" s="71"/>
+      <c r="B38" s="72"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -3853,8 +3889,8 @@
         <v>5.5975999999999998E-2</v>
       </c>
       <c r="J38" s="24"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="72"/>
       <c r="M38" s="16" t="s">
         <v>25</v>
       </c>
@@ -3875,8 +3911,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="70"/>
-      <c r="B39" s="71"/>
+      <c r="A39" s="71"/>
+      <c r="B39" s="72"/>
       <c r="C39" s="16" t="s">
         <v>26</v>
       </c>
@@ -3895,8 +3931,8 @@
       <c r="H39" s="16">
         <v>2.3768000000000001E-2</v>
       </c>
-      <c r="K39" s="70"/>
-      <c r="L39" s="71"/>
+      <c r="K39" s="71"/>
+      <c r="L39" s="72"/>
       <c r="M39" s="16" t="s">
         <v>26</v>
       </c>
@@ -3917,8 +3953,8 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="72"/>
-      <c r="B40" s="73"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="74"/>
       <c r="C40" s="19" t="s">
         <v>32</v>
       </c>
@@ -3942,8 +3978,8 @@
         <f t="shared" si="6"/>
         <v>7.9743999999999995E-2</v>
       </c>
-      <c r="K40" s="72"/>
-      <c r="L40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="74"/>
       <c r="M40" s="19" t="s">
         <v>32</v>
       </c>
@@ -3969,10 +4005,10 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="53">
+      <c r="A41" s="75">
         <v>1280</v>
       </c>
-      <c r="B41" s="54"/>
+      <c r="B41" s="76"/>
       <c r="C41" s="4" t="s">
         <v>23</v>
       </c>
@@ -3990,10 +4026,10 @@
       </c>
       <c r="H41" s="5"/>
       <c r="J41" s="24"/>
-      <c r="K41" s="53">
+      <c r="K41" s="75">
         <v>1280</v>
       </c>
-      <c r="L41" s="54"/>
+      <c r="L41" s="76"/>
       <c r="M41" s="4" t="s">
         <v>23</v>
       </c>
@@ -4014,8 +4050,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="55"/>
-      <c r="B42" s="56"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
@@ -4032,8 +4068,8 @@
         <v>9.476E-3</v>
       </c>
       <c r="H42" s="5"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="56"/>
+      <c r="K42" s="77"/>
+      <c r="L42" s="78"/>
       <c r="M42" s="4" t="s">
         <v>24</v>
       </c>
@@ -4054,8 +4090,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="55"/>
-      <c r="B43" s="56"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="78"/>
       <c r="C43" s="19" t="s">
         <v>32</v>
       </c>
@@ -4076,8 +4112,8 @@
         <v>2.7875999999999998E-2</v>
       </c>
       <c r="H43" s="5"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="56"/>
+      <c r="K43" s="77"/>
+      <c r="L43" s="78"/>
       <c r="M43" s="19" t="s">
         <v>32</v>
       </c>
@@ -4103,8 +4139,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="55"/>
-      <c r="B44" s="56"/>
+      <c r="A44" s="77"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
@@ -4122,8 +4158,8 @@
       </c>
       <c r="H44" s="5"/>
       <c r="J44" s="24"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="56"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="78"/>
       <c r="M44" s="4" t="s">
         <v>25</v>
       </c>
@@ -4144,8 +4180,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="55"/>
-      <c r="B45" s="56"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="78"/>
       <c r="C45" s="4" t="s">
         <v>26</v>
       </c>
@@ -4162,8 +4198,8 @@
         <v>4.3580000000000001E-2</v>
       </c>
       <c r="H45" s="5"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="56"/>
+      <c r="K45" s="77"/>
+      <c r="L45" s="78"/>
       <c r="M45" s="4" t="s">
         <v>26</v>
       </c>
@@ -4184,8 +4220,8 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="57"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="79"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="19" t="s">
         <v>32</v>
       </c>
@@ -4206,8 +4242,8 @@
         <v>0.146428</v>
       </c>
       <c r="H46" s="5"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="58"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="80"/>
       <c r="M46" s="19" t="s">
         <v>32</v>
       </c>
@@ -4233,10 +4269,10 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="74">
+      <c r="A47" s="56">
         <v>1345</v>
       </c>
-      <c r="B47" s="75"/>
+      <c r="B47" s="57"/>
       <c r="C47" s="7" t="s">
         <v>23</v>
       </c>
@@ -4254,10 +4290,10 @@
       </c>
       <c r="H47" s="5"/>
       <c r="J47" s="24"/>
-      <c r="K47" s="74">
+      <c r="K47" s="56">
         <v>1345</v>
       </c>
-      <c r="L47" s="75"/>
+      <c r="L47" s="57"/>
       <c r="M47" s="7" t="s">
         <v>23</v>
       </c>
@@ -4278,8 +4314,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="76"/>
-      <c r="B48" s="77"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="59"/>
       <c r="C48" s="7" t="s">
         <v>24</v>
       </c>
@@ -4296,8 +4332,8 @@
         <v>9.9319999999999999E-3</v>
       </c>
       <c r="H48" s="5"/>
-      <c r="K48" s="76"/>
-      <c r="L48" s="77"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="59"/>
       <c r="M48" s="7" t="s">
         <v>24</v>
       </c>
@@ -4316,8 +4352,8 @@
       <c r="R48" s="5"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="76"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="59"/>
       <c r="C49" s="19" t="s">
         <v>32</v>
       </c>
@@ -4338,8 +4374,8 @@
         <v>2.8931999999999999E-2</v>
       </c>
       <c r="H49" s="5"/>
-      <c r="K49" s="76"/>
-      <c r="L49" s="77"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="59"/>
       <c r="M49" s="19" t="s">
         <v>32</v>
       </c>
@@ -4362,8 +4398,8 @@
       <c r="R49" s="5"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="76"/>
-      <c r="B50" s="77"/>
+      <c r="A50" s="58"/>
+      <c r="B50" s="59"/>
       <c r="C50" s="7" t="s">
         <v>25</v>
       </c>
@@ -4381,8 +4417,8 @@
       </c>
       <c r="H50" s="5"/>
       <c r="J50" s="24"/>
-      <c r="K50" s="76"/>
-      <c r="L50" s="77"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="59"/>
       <c r="M50" s="7" t="s">
         <v>25</v>
       </c>
@@ -4401,8 +4437,8 @@
       <c r="R50" s="5"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="76"/>
-      <c r="B51" s="77"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="59"/>
       <c r="C51" s="7" t="s">
         <v>26</v>
       </c>
@@ -4419,8 +4455,8 @@
         <v>4.5887999999999998E-2</v>
       </c>
       <c r="H51" s="5"/>
-      <c r="K51" s="76"/>
-      <c r="L51" s="77"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="59"/>
       <c r="M51" s="7" t="s">
         <v>26</v>
       </c>
@@ -4439,8 +4475,8 @@
       <c r="R51" s="5"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="78"/>
-      <c r="B52" s="79"/>
+      <c r="A52" s="60"/>
+      <c r="B52" s="61"/>
       <c r="C52" s="19" t="s">
         <v>32</v>
       </c>
@@ -4461,8 +4497,8 @@
         <v>0.15465999999999999</v>
       </c>
       <c r="H52" s="5"/>
-      <c r="K52" s="78"/>
-      <c r="L52" s="79"/>
+      <c r="K52" s="60"/>
+      <c r="L52" s="61"/>
       <c r="M52" s="19" t="s">
         <v>32</v>
       </c>
@@ -4486,6 +4522,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K41:L46"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L8"/>
+    <mergeCell ref="K9:L13"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="K47:L52"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="A47:B52"/>
@@ -4502,13 +4545,6 @@
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="K29:L34"/>
     <mergeCell ref="K35:L40"/>
-    <mergeCell ref="K41:L46"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L8"/>
-    <mergeCell ref="K9:L13"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4546,32 +4582,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="61"/>
+      <c r="B2" s="82"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15" t="s">
         <v>1</v>
@@ -4623,10 +4659,10 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="62">
+      <c r="A3" s="63">
         <v>584</v>
       </c>
-      <c r="B3" s="63"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -4680,8 +4716,8 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
@@ -4735,8 +4771,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="65"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -4806,8 +4842,8 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4861,8 +4897,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="67"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
@@ -4932,10 +4968,10 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="68">
+      <c r="A8" s="69">
         <v>980</v>
       </c>
-      <c r="B8" s="69"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="16" t="s">
         <v>30</v>
       </c>
@@ -4986,8 +5022,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="70"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
@@ -5041,8 +5077,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="16" t="s">
         <v>35</v>
       </c>
@@ -5108,8 +5144,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="71"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="16" t="s">
         <v>22</v>
       </c>
@@ -5163,8 +5199,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="16" t="s">
         <v>34</v>
       </c>
@@ -5230,10 +5266,10 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="53">
+      <c r="A13" s="75">
         <v>1280</v>
       </c>
-      <c r="B13" s="54"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
@@ -5284,8 +5320,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="56"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
@@ -5339,8 +5375,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="56"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
@@ -5406,8 +5442,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
@@ -5461,8 +5497,8 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="58"/>
+      <c r="A17" s="79"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
@@ -5528,10 +5564,10 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="74">
+      <c r="A18" s="56">
         <v>1345</v>
       </c>
-      <c r="B18" s="75"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="7" t="s">
         <v>30</v>
       </c>
@@ -5585,8 +5621,8 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="76"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
@@ -5643,8 +5679,8 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="76"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="7" t="s">
         <v>35</v>
       </c>
@@ -5710,8 +5746,8 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
@@ -5765,8 +5801,8 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="78"/>
-      <c r="B22" s="79"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -5832,10 +5868,10 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="81">
+      <c r="A23" s="84">
         <v>1640</v>
       </c>
-      <c r="B23" s="82"/>
+      <c r="B23" s="85"/>
       <c r="C23" s="39" t="s">
         <v>30</v>
       </c>
@@ -5866,8 +5902,8 @@
       <c r="R23" s="40"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="84"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="87"/>
       <c r="C24" s="39" t="s">
         <v>21</v>
       </c>
@@ -5899,8 +5935,8 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
-      <c r="B25" s="84"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="87"/>
       <c r="C25" s="39" t="s">
         <v>35</v>
       </c>
@@ -5963,8 +5999,8 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
-      <c r="B26" s="84"/>
+      <c r="A26" s="86"/>
+      <c r="B26" s="87"/>
       <c r="C26" s="39" t="s">
         <v>22</v>
       </c>
@@ -5996,8 +6032,8 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="85"/>
-      <c r="B27" s="86"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="89"/>
       <c r="C27" s="39" t="s">
         <v>34</v>
       </c>
@@ -6071,10 +6107,10 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="61"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="14"/>
       <c r="D33" s="15" t="s">
         <v>1</v>
@@ -6123,10 +6159,10 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="62">
+      <c r="A34" s="63">
         <v>584</v>
       </c>
-      <c r="B34" s="63"/>
+      <c r="B34" s="64"/>
       <c r="C34" s="1" t="s">
         <v>23</v>
       </c>
@@ -6177,8 +6213,8 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="64"/>
-      <c r="B35" s="65"/>
+      <c r="A35" s="65"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
@@ -6229,8 +6265,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="64"/>
-      <c r="B36" s="65"/>
+      <c r="A36" s="65"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="19" t="s">
         <v>32</v>
       </c>
@@ -6296,8 +6332,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="64"/>
-      <c r="B37" s="65"/>
+      <c r="A37" s="65"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
@@ -6348,8 +6384,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="64"/>
-      <c r="B38" s="65"/>
+      <c r="A38" s="65"/>
+      <c r="B38" s="66"/>
       <c r="C38" s="1" t="s">
         <v>26</v>
       </c>
@@ -6400,8 +6436,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="66"/>
-      <c r="B39" s="67"/>
+      <c r="A39" s="67"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="19" t="s">
         <v>32</v>
       </c>
@@ -6467,10 +6503,10 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="68">
+      <c r="A40" s="69">
         <v>980</v>
       </c>
-      <c r="B40" s="69"/>
+      <c r="B40" s="70"/>
       <c r="C40" s="16" t="s">
         <v>23</v>
       </c>
@@ -6521,8 +6557,8 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="70"/>
-      <c r="B41" s="71"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="16" t="s">
         <v>24</v>
       </c>
@@ -6573,8 +6609,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="70"/>
-      <c r="B42" s="71"/>
+      <c r="A42" s="71"/>
+      <c r="B42" s="72"/>
       <c r="C42" s="19" t="s">
         <v>32</v>
       </c>
@@ -6640,8 +6676,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="70"/>
-      <c r="B43" s="71"/>
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
       <c r="C43" s="16" t="s">
         <v>25</v>
       </c>
@@ -6692,8 +6728,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="70"/>
-      <c r="B44" s="71"/>
+      <c r="A44" s="71"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="16" t="s">
         <v>26</v>
       </c>
@@ -6744,8 +6780,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="72"/>
-      <c r="B45" s="73"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="74"/>
       <c r="C45" s="19" t="s">
         <v>32</v>
       </c>
@@ -6811,10 +6847,10 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="53">
+      <c r="A46" s="75">
         <v>1280</v>
       </c>
-      <c r="B46" s="54"/>
+      <c r="B46" s="76"/>
       <c r="C46" s="4" t="s">
         <v>23</v>
       </c>
@@ -6865,8 +6901,8 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="55"/>
-      <c r="B47" s="56"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="78"/>
       <c r="C47" s="4" t="s">
         <v>24</v>
       </c>
@@ -6917,8 +6953,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="55"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="77"/>
+      <c r="B48" s="78"/>
       <c r="C48" s="19" t="s">
         <v>32</v>
       </c>
@@ -6984,8 +7020,8 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="55"/>
-      <c r="B49" s="56"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="78"/>
       <c r="C49" s="4" t="s">
         <v>25</v>
       </c>
@@ -7036,8 +7072,8 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="55"/>
-      <c r="B50" s="56"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="78"/>
       <c r="C50" s="4" t="s">
         <v>26</v>
       </c>
@@ -7088,8 +7124,8 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
-      <c r="B51" s="58"/>
+      <c r="A51" s="79"/>
+      <c r="B51" s="80"/>
       <c r="C51" s="19" t="s">
         <v>32</v>
       </c>
@@ -7155,10 +7191,10 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="74">
+      <c r="A52" s="56">
         <v>1345</v>
       </c>
-      <c r="B52" s="75"/>
+      <c r="B52" s="57"/>
       <c r="C52" s="7" t="s">
         <v>23</v>
       </c>
@@ -7209,8 +7245,8 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="76"/>
-      <c r="B53" s="77"/>
+      <c r="A53" s="58"/>
+      <c r="B53" s="59"/>
       <c r="C53" s="7" t="s">
         <v>24</v>
       </c>
@@ -7261,8 +7297,8 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="76"/>
-      <c r="B54" s="77"/>
+      <c r="A54" s="58"/>
+      <c r="B54" s="59"/>
       <c r="C54" s="19" t="s">
         <v>32</v>
       </c>
@@ -7328,8 +7364,8 @@
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="76"/>
-      <c r="B55" s="77"/>
+      <c r="A55" s="58"/>
+      <c r="B55" s="59"/>
       <c r="C55" s="7" t="s">
         <v>25</v>
       </c>
@@ -7380,8 +7416,8 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="76"/>
-      <c r="B56" s="77"/>
+      <c r="A56" s="58"/>
+      <c r="B56" s="59"/>
       <c r="C56" s="7" t="s">
         <v>26</v>
       </c>
@@ -7432,8 +7468,8 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="78"/>
-      <c r="B57" s="79"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="61"/>
       <c r="C57" s="19" t="s">
         <v>32</v>
       </c>
@@ -7759,29 +7795,29 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="93" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="88"/>
-      <c r="E15" s="87" t="s">
+      <c r="D15" s="93"/>
+      <c r="E15" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="89" t="s">
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="94"/>
+      <c r="O15" s="90" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="42">
         <v>1</v>
       </c>
@@ -7812,10 +7848,10 @@
       <c r="N16" s="42">
         <v>10</v>
       </c>
-      <c r="O16" s="89"/>
+      <c r="O16" s="90"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="89" t="s">
+      <c r="C17" s="90" t="s">
         <v>96</v>
       </c>
       <c r="D17" s="42" t="s">
@@ -7851,13 +7887,13 @@
       <c r="N17" s="43">
         <v>41</v>
       </c>
-      <c r="O17" s="90">
+      <c r="O17" s="91">
         <f>SUM(E17:N17)/410</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="89"/>
+      <c r="C18" s="90"/>
       <c r="D18" s="42" t="s">
         <v>98</v>
       </c>
@@ -7891,32 +7927,32 @@
       <c r="N18" s="43">
         <v>0</v>
       </c>
-      <c r="O18" s="91"/>
+      <c r="O18" s="92"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="88" t="s">
+      <c r="C21" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="88"/>
-      <c r="E21" s="87" t="s">
+      <c r="D21" s="93"/>
+      <c r="E21" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="87"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="87"/>
-      <c r="M21" s="87"/>
-      <c r="N21" s="87"/>
-      <c r="O21" s="89" t="s">
+      <c r="F21" s="94"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="94"/>
+      <c r="M21" s="94"/>
+      <c r="N21" s="94"/>
+      <c r="O21" s="90" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
       <c r="E22" s="42">
         <v>1</v>
       </c>
@@ -7947,10 +7983,10 @@
       <c r="N22" s="42">
         <v>10</v>
       </c>
-      <c r="O22" s="89"/>
+      <c r="O22" s="90"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="89" t="s">
+      <c r="C23" s="90" t="s">
         <v>96</v>
       </c>
       <c r="D23" s="42" t="s">
@@ -7986,13 +8022,13 @@
       <c r="N23" s="35">
         <v>27</v>
       </c>
-      <c r="O23" s="90">
+      <c r="O23" s="91">
         <f>SUM(E23:N23)/410</f>
         <v>0.86829268292682926</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="89"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="42" t="s">
         <v>98</v>
       </c>
@@ -8026,32 +8062,32 @@
       <c r="N24" s="43">
         <v>14</v>
       </c>
-      <c r="O24" s="91"/>
+      <c r="O24" s="92"/>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="87" t="s">
+      <c r="D27" s="93"/>
+      <c r="E27" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="87"/>
-      <c r="O27" s="89" t="s">
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="94"/>
+      <c r="M27" s="94"/>
+      <c r="N27" s="94"/>
+      <c r="O27" s="90" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="88"/>
-      <c r="D28" s="88"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="93"/>
       <c r="E28" s="42">
         <v>1</v>
       </c>
@@ -8082,10 +8118,10 @@
       <c r="N28" s="42">
         <v>10</v>
       </c>
-      <c r="O28" s="89"/>
+      <c r="O28" s="90"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="89" t="s">
+      <c r="C29" s="90" t="s">
         <v>96</v>
       </c>
       <c r="D29" s="42" t="s">
@@ -8121,13 +8157,13 @@
       <c r="N29" s="35">
         <v>29</v>
       </c>
-      <c r="O29" s="90">
+      <c r="O29" s="91">
         <f>SUM(E29:N29)/410</f>
         <v>0.69512195121951215</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="89"/>
+      <c r="C30" s="90"/>
       <c r="D30" s="42" t="s">
         <v>98</v>
       </c>
@@ -8161,7 +8197,7 @@
       <c r="N30" s="43">
         <v>12</v>
       </c>
-      <c r="O30" s="91"/>
+      <c r="O30" s="92"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="46"/>
@@ -8210,6 +8246,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E15:N15"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="O29:O30"/>
     <mergeCell ref="C21:D22"/>
@@ -8220,11 +8261,6 @@
     <mergeCell ref="C27:D28"/>
     <mergeCell ref="E27:N27"/>
     <mergeCell ref="O27:O28"/>
-    <mergeCell ref="E15:N15"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8234,61 +8270,82 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AD41"/>
+  <dimension ref="A4:AN41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="33" max="33" width="9" customWidth="1"/>
+    <col min="34" max="34" width="9.7109375" customWidth="1"/>
+    <col min="35" max="35" width="8.28515625" customWidth="1"/>
+    <col min="36" max="37" width="8.5703125" customWidth="1"/>
+    <col min="38" max="38" width="8.42578125" customWidth="1"/>
+    <col min="39" max="39" width="8.28515625" customWidth="1"/>
+    <col min="40" max="40" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="87" t="s">
+    <row r="4" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="93"/>
+      <c r="D4" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="89" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="R4" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="S4" s="93"/>
+      <c r="T4" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="U4" s="94"/>
+      <c r="V4" s="94"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="94"/>
+      <c r="AD4" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="R4" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="S4" s="88"/>
-      <c r="T4" s="87" t="s">
-        <v>100</v>
-      </c>
-      <c r="U4" s="87"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="89" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
+      <c r="AG4" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH4" s="94" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI4" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="94"/>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+    </row>
+    <row r="5" spans="2:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="45">
         <v>1</v>
       </c>
@@ -8319,9 +8376,9 @@
       <c r="M5" s="45">
         <v>10</v>
       </c>
-      <c r="N5" s="89"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
+      <c r="N5" s="90"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
       <c r="T5" s="45">
         <v>1</v>
       </c>
@@ -8352,11 +8409,31 @@
       <c r="AC5" s="45">
         <v>10</v>
       </c>
-      <c r="AD5" s="89"/>
-    </row>
-    <row r="6" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="87" t="s">
-        <v>107</v>
+      <c r="AD5" s="90"/>
+      <c r="AG5" s="90"/>
+      <c r="AH5" s="94"/>
+      <c r="AI5" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL5" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM5" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN5" s="53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>1</v>
@@ -8405,8 +8482,8 @@
         <f>AVERAGE(D6:M6)</f>
         <v>9.2636986301369864E-2</v>
       </c>
-      <c r="R6" s="87" t="s">
-        <v>108</v>
+      <c r="R6" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="S6" s="45" t="s">
         <v>1</v>
@@ -8445,9 +8522,39 @@
         <f>AVERAGE(T6:AC6)</f>
         <v>5.8035200000000009E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="87"/>
+      <c r="AG6" s="53">
+        <v>584</v>
+      </c>
+      <c r="AH6" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI6" s="110">
+        <f>AD6</f>
+        <v>5.8035200000000009E-2</v>
+      </c>
+      <c r="AJ6" s="110">
+        <f>AD7</f>
+        <v>4.6922399999999996E-2</v>
+      </c>
+      <c r="AK6" s="110">
+        <f>AD8</f>
+        <v>4.1415600000000004E-2</v>
+      </c>
+      <c r="AL6" s="110">
+        <f>AD9</f>
+        <v>3.2311600000000003E-2</v>
+      </c>
+      <c r="AM6" s="110">
+        <f>AD10</f>
+        <v>2.9476800000000004E-2</v>
+      </c>
+      <c r="AN6" s="110">
+        <f>AD11</f>
+        <v>3.0045600000000006E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B7" s="112"/>
       <c r="C7" s="45" t="s">
         <v>2</v>
       </c>
@@ -8495,7 +8602,7 @@
         <f t="shared" ref="N7:N11" si="0">AVERAGE(D7:M7)</f>
         <v>0.2441780821917808</v>
       </c>
-      <c r="R7" s="87"/>
+      <c r="R7" s="112"/>
       <c r="S7" s="45" t="s">
         <v>2</v>
       </c>
@@ -8533,9 +8640,39 @@
         <f t="shared" ref="AD7:AD11" si="1">AVERAGE(T7:AC7)</f>
         <v>4.6922399999999996E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="87"/>
+      <c r="AG7" s="53">
+        <v>980</v>
+      </c>
+      <c r="AH7" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI7" s="43">
+        <f>AD16</f>
+        <v>9.6875600000000006E-2</v>
+      </c>
+      <c r="AJ7" s="43">
+        <f>AD17</f>
+        <v>8.1484000000000001E-2</v>
+      </c>
+      <c r="AK7" s="43">
+        <f>AD18</f>
+        <v>6.8795999999999996E-2</v>
+      </c>
+      <c r="AL7" s="43">
+        <f>AD19</f>
+        <v>5.4722799999999995E-2</v>
+      </c>
+      <c r="AM7" s="43">
+        <f>AD20</f>
+        <v>5.2898399999999998E-2</v>
+      </c>
+      <c r="AN7" s="43">
+        <f>AD21</f>
+        <v>4.9896800000000005E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B8" s="112"/>
       <c r="C8" s="45" t="s">
         <v>3</v>
       </c>
@@ -8583,7 +8720,7 @@
         <f t="shared" si="0"/>
         <v>0.31849315068493156</v>
       </c>
-      <c r="R8" s="87"/>
+      <c r="R8" s="112"/>
       <c r="S8" s="45" t="s">
         <v>3</v>
       </c>
@@ -8621,9 +8758,39 @@
         <f t="shared" si="1"/>
         <v>4.1415600000000004E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B9" s="87"/>
+      <c r="AG8" s="53">
+        <v>1280</v>
+      </c>
+      <c r="AH8" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI8" s="43">
+        <f>AD26</f>
+        <v>0.12733359999999999</v>
+      </c>
+      <c r="AJ8" s="43">
+        <f>AD27</f>
+        <v>0.11091480000000001</v>
+      </c>
+      <c r="AK8" s="43">
+        <f>AD28</f>
+        <v>8.7704799999999999E-2</v>
+      </c>
+      <c r="AL8" s="43">
+        <f>AD29</f>
+        <v>7.7805600000000003E-2</v>
+      </c>
+      <c r="AM8" s="43">
+        <f>AD30</f>
+        <v>7.8400400000000009E-2</v>
+      </c>
+      <c r="AN8" s="54" t="str">
+        <f>AD31</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="9" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B9" s="112"/>
       <c r="C9" s="45" t="s">
         <v>52</v>
       </c>
@@ -8671,7 +8838,7 @@
         <f t="shared" si="0"/>
         <v>0.49383561643835616</v>
       </c>
-      <c r="R9" s="87"/>
+      <c r="R9" s="112"/>
       <c r="S9" s="45" t="s">
         <v>52</v>
       </c>
@@ -8709,9 +8876,39 @@
         <f t="shared" si="1"/>
         <v>3.2311600000000003E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="87"/>
+      <c r="AG9" s="53">
+        <v>1345</v>
+      </c>
+      <c r="AH9" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI9" s="43">
+        <f>AD36</f>
+        <v>0.1336464</v>
+      </c>
+      <c r="AJ9" s="43">
+        <f>AD37</f>
+        <v>0.11642079999999999</v>
+      </c>
+      <c r="AK9" s="43">
+        <f>AD38</f>
+        <v>9.1741199999999995E-2</v>
+      </c>
+      <c r="AL9" s="43">
+        <f>AD39</f>
+        <v>8.16828E-2</v>
+      </c>
+      <c r="AM9" s="43">
+        <f>AD40</f>
+        <v>8.2377599999999995E-2</v>
+      </c>
+      <c r="AN9" s="54" t="str">
+        <f>AD41</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="10" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B10" s="112"/>
       <c r="C10" s="45" t="s">
         <v>51</v>
       </c>
@@ -8759,7 +8956,7 @@
         <f t="shared" si="0"/>
         <v>0.59845890410958913</v>
       </c>
-      <c r="R10" s="87"/>
+      <c r="R10" s="112"/>
       <c r="S10" s="45" t="s">
         <v>51</v>
       </c>
@@ -8798,8 +8995,8 @@
         <v>2.9476800000000004E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B11" s="87"/>
+    <row r="11" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B11" s="112"/>
       <c r="C11" s="45" t="s">
         <v>69</v>
       </c>
@@ -8847,7 +9044,7 @@
         <f t="shared" si="0"/>
         <v>0.56746575342465744</v>
       </c>
-      <c r="R11" s="87"/>
+      <c r="R11" s="112"/>
       <c r="S11" s="45" t="s">
         <v>69</v>
       </c>
@@ -8886,49 +9083,63 @@
         <v>3.0045600000000006E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B14" s="88" t="s">
+    <row r="14" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B14" s="93" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="93"/>
+      <c r="D14" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="94"/>
+      <c r="N14" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="R14" s="93" t="s">
+        <v>118</v>
+      </c>
+      <c r="S14" s="93"/>
+      <c r="T14" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="U14" s="94"/>
+      <c r="V14" s="94"/>
+      <c r="W14" s="94"/>
+      <c r="X14" s="94"/>
+      <c r="Y14" s="94"/>
+      <c r="Z14" s="94"/>
+      <c r="AA14" s="94"/>
+      <c r="AB14" s="94"/>
+      <c r="AC14" s="94"/>
+      <c r="AD14" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG14" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH14" s="94" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="88"/>
-      <c r="D14" s="87" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="87"/>
-      <c r="K14" s="87"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="89" t="s">
-        <v>105</v>
-      </c>
-      <c r="R14" s="88" t="s">
-        <v>109</v>
-      </c>
-      <c r="S14" s="88"/>
-      <c r="T14" s="87" t="s">
-        <v>100</v>
-      </c>
-      <c r="U14" s="87"/>
-      <c r="V14" s="87"/>
-      <c r="W14" s="87"/>
-      <c r="X14" s="87"/>
-      <c r="Y14" s="87"/>
-      <c r="Z14" s="87"/>
-      <c r="AA14" s="87"/>
-      <c r="AB14" s="87"/>
-      <c r="AC14" s="87"/>
-      <c r="AD14" s="89" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
+      <c r="AI14" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ14" s="94"/>
+      <c r="AK14" s="94"/>
+      <c r="AL14" s="94"/>
+      <c r="AM14" s="94"/>
+      <c r="AN14" s="94"/>
+    </row>
+    <row r="15" spans="2:40" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="45">
         <v>1</v>
       </c>
@@ -8959,9 +9170,9 @@
       <c r="M15" s="45">
         <v>10</v>
       </c>
-      <c r="N15" s="89"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="88"/>
+      <c r="N15" s="90"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
       <c r="T15" s="45">
         <v>1</v>
       </c>
@@ -8992,11 +9203,31 @@
       <c r="AC15" s="45">
         <v>10</v>
       </c>
-      <c r="AD15" s="89"/>
-    </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="87" t="s">
-        <v>107</v>
+      <c r="AD15" s="90"/>
+      <c r="AG15" s="90"/>
+      <c r="AH15" s="94"/>
+      <c r="AI15" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL15" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM15" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN15" s="53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B16" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="C16" s="45" t="s">
         <v>1</v>
@@ -9045,8 +9276,8 @@
         <f>AVERAGE(D16:M16)</f>
         <v>9.5918367346938788E-2</v>
       </c>
-      <c r="R16" s="87" t="s">
-        <v>108</v>
+      <c r="R16" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="S16" s="45" t="s">
         <v>1</v>
@@ -9085,9 +9316,39 @@
         <f>AVERAGE(T16:AC16)</f>
         <v>9.6875600000000006E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B17" s="87"/>
+      <c r="AG16" s="53">
+        <v>584</v>
+      </c>
+      <c r="AH16" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI16" s="111">
+        <f>N6</f>
+        <v>9.2636986301369864E-2</v>
+      </c>
+      <c r="AJ16" s="111">
+        <f>N7</f>
+        <v>0.2441780821917808</v>
+      </c>
+      <c r="AK16" s="111">
+        <f>N8</f>
+        <v>0.31849315068493156</v>
+      </c>
+      <c r="AL16" s="111">
+        <f>N9</f>
+        <v>0.49383561643835616</v>
+      </c>
+      <c r="AM16" s="111">
+        <f>N10</f>
+        <v>0.59845890410958913</v>
+      </c>
+      <c r="AN16" s="111">
+        <f>N11</f>
+        <v>0.56746575342465744</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B17" s="112"/>
       <c r="C17" s="45" t="s">
         <v>2</v>
       </c>
@@ -9135,7 +9396,7 @@
         <f t="shared" ref="N17:N21" si="2">AVERAGE(D17:M17)</f>
         <v>0.19918367346938778</v>
       </c>
-      <c r="R17" s="87"/>
+      <c r="R17" s="112"/>
       <c r="S17" s="45" t="s">
         <v>2</v>
       </c>
@@ -9173,9 +9434,39 @@
         <f t="shared" ref="AD17:AD21" si="3">AVERAGE(T17:AC17)</f>
         <v>8.1484000000000001E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B18" s="87"/>
+      <c r="AG17" s="53">
+        <v>980</v>
+      </c>
+      <c r="AH17" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI17" s="109">
+        <f>N16</f>
+        <v>9.5918367346938788E-2</v>
+      </c>
+      <c r="AJ17" s="109">
+        <f>N17</f>
+        <v>0.19918367346938778</v>
+      </c>
+      <c r="AK17" s="109">
+        <f>N18</f>
+        <v>0.32346938775510203</v>
+      </c>
+      <c r="AL17" s="109">
+        <f>N19</f>
+        <v>0.49091836734693883</v>
+      </c>
+      <c r="AM17" s="109">
+        <f>N20</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="AN17" s="109">
+        <f>N21</f>
+        <v>0.60499999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B18" s="112"/>
       <c r="C18" s="45" t="s">
         <v>3</v>
       </c>
@@ -9223,7 +9514,7 @@
         <f t="shared" si="2"/>
         <v>0.32346938775510203</v>
       </c>
-      <c r="R18" s="87"/>
+      <c r="R18" s="112"/>
       <c r="S18" s="45" t="s">
         <v>3</v>
       </c>
@@ -9261,9 +9552,39 @@
         <f t="shared" si="3"/>
         <v>6.8795999999999996E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B19" s="87"/>
+      <c r="AG18" s="53">
+        <v>1280</v>
+      </c>
+      <c r="AH18" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI18" s="109">
+        <f>N26</f>
+        <v>0.10015624999999999</v>
+      </c>
+      <c r="AJ18" s="109">
+        <f>N27</f>
+        <v>0.16820312499999998</v>
+      </c>
+      <c r="AK18" s="109">
+        <f>N28</f>
+        <v>0.37398437499999998</v>
+      </c>
+      <c r="AL18" s="109">
+        <f>N29</f>
+        <v>0.45929687499999999</v>
+      </c>
+      <c r="AM18" s="109">
+        <f>N30</f>
+        <v>0.50226562500000005</v>
+      </c>
+      <c r="AN18" s="54" t="str">
+        <f>AD41</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B19" s="112"/>
       <c r="C19" s="45" t="s">
         <v>52</v>
       </c>
@@ -9311,7 +9632,7 @@
         <f t="shared" si="2"/>
         <v>0.49091836734693883</v>
       </c>
-      <c r="R19" s="87"/>
+      <c r="R19" s="112"/>
       <c r="S19" s="45" t="s">
         <v>52</v>
       </c>
@@ -9349,9 +9670,39 @@
         <f t="shared" si="3"/>
         <v>5.4722799999999995E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B20" s="87"/>
+      <c r="AG19" s="53">
+        <v>1345</v>
+      </c>
+      <c r="AH19" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI19" s="109">
+        <f>N36</f>
+        <v>0.10200743494423789</v>
+      </c>
+      <c r="AJ19" s="109">
+        <f>N37</f>
+        <v>0.16988847583643124</v>
+      </c>
+      <c r="AK19" s="109">
+        <f>N38</f>
+        <v>0.37724907063197022</v>
+      </c>
+      <c r="AL19" s="109">
+        <f>N39</f>
+        <v>0.45933085501858739</v>
+      </c>
+      <c r="AM19" s="109">
+        <f>N40</f>
+        <v>0.54542750929368033</v>
+      </c>
+      <c r="AN19" s="54">
+        <f>AD51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B20" s="112"/>
       <c r="C20" s="45" t="s">
         <v>51</v>
       </c>
@@ -9399,7 +9750,7 @@
         <f t="shared" si="2"/>
         <v>0.54499999999999993</v>
       </c>
-      <c r="R20" s="87"/>
+      <c r="R20" s="112"/>
       <c r="S20" s="45" t="s">
         <v>51</v>
       </c>
@@ -9438,8 +9789,8 @@
         <v>5.2898399999999998E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B21" s="87"/>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B21" s="112"/>
       <c r="C21" s="45" t="s">
         <v>69</v>
       </c>
@@ -9487,7 +9838,7 @@
         <f t="shared" si="2"/>
         <v>0.60499999999999998</v>
       </c>
-      <c r="R21" s="87"/>
+      <c r="R21" s="112"/>
       <c r="S21" s="45" t="s">
         <v>69</v>
       </c>
@@ -9526,49 +9877,49 @@
         <v>4.9896800000000005E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B24" s="88" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="87" t="s">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B24" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="93"/>
+      <c r="D24" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="89" t="s">
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="94"/>
+      <c r="M24" s="94"/>
+      <c r="N24" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="R24" s="88" t="s">
-        <v>110</v>
-      </c>
-      <c r="S24" s="88"/>
-      <c r="T24" s="87" t="s">
+      <c r="R24" s="93" t="s">
+        <v>119</v>
+      </c>
+      <c r="S24" s="93"/>
+      <c r="T24" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="U24" s="87"/>
-      <c r="V24" s="87"/>
-      <c r="W24" s="87"/>
-      <c r="X24" s="87"/>
-      <c r="Y24" s="87"/>
-      <c r="Z24" s="87"/>
-      <c r="AA24" s="87"/>
-      <c r="AB24" s="87"/>
-      <c r="AC24" s="87"/>
-      <c r="AD24" s="89" t="s">
+      <c r="U24" s="94"/>
+      <c r="V24" s="94"/>
+      <c r="W24" s="94"/>
+      <c r="X24" s="94"/>
+      <c r="Y24" s="94"/>
+      <c r="Z24" s="94"/>
+      <c r="AA24" s="94"/>
+      <c r="AB24" s="94"/>
+      <c r="AC24" s="94"/>
+      <c r="AD24" s="90" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
+    <row r="25" spans="1:40" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="93"/>
+      <c r="C25" s="93"/>
       <c r="D25" s="45">
         <v>1</v>
       </c>
@@ -9599,9 +9950,9 @@
       <c r="M25" s="45">
         <v>10</v>
       </c>
-      <c r="N25" s="89"/>
-      <c r="R25" s="88"/>
-      <c r="S25" s="88"/>
+      <c r="N25" s="90"/>
+      <c r="R25" s="93"/>
+      <c r="S25" s="93"/>
       <c r="T25" s="45">
         <v>1</v>
       </c>
@@ -9632,11 +9983,11 @@
       <c r="AC25" s="45">
         <v>10</v>
       </c>
-      <c r="AD25" s="89"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B26" s="87" t="s">
-        <v>107</v>
+      <c r="AD25" s="90"/>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B26" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="C26" s="45" t="s">
         <v>1</v>
@@ -9685,8 +10036,8 @@
         <f>AVERAGE(D26:M26)</f>
         <v>0.10015624999999999</v>
       </c>
-      <c r="R26" s="87" t="s">
-        <v>108</v>
+      <c r="R26" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="S26" s="45" t="s">
         <v>1</v>
@@ -9726,8 +10077,8 @@
         <v>0.12733359999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B27" s="87"/>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B27" s="112"/>
       <c r="C27" s="45" t="s">
         <v>2</v>
       </c>
@@ -9775,7 +10126,7 @@
         <f t="shared" ref="N27:N31" si="4">AVERAGE(D27:M27)</f>
         <v>0.16820312499999998</v>
       </c>
-      <c r="R27" s="87"/>
+      <c r="R27" s="112"/>
       <c r="S27" s="45" t="s">
         <v>2</v>
       </c>
@@ -9814,8 +10165,8 @@
         <v>0.11091480000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B28" s="87"/>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B28" s="112"/>
       <c r="C28" s="45" t="s">
         <v>3</v>
       </c>
@@ -9863,7 +10214,7 @@
         <f t="shared" si="4"/>
         <v>0.37398437499999998</v>
       </c>
-      <c r="R28" s="87"/>
+      <c r="R28" s="112"/>
       <c r="S28" s="45" t="s">
         <v>3</v>
       </c>
@@ -9902,8 +10253,8 @@
         <v>8.7704799999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B29" s="87"/>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B29" s="112"/>
       <c r="C29" s="45" t="s">
         <v>52</v>
       </c>
@@ -9951,7 +10302,7 @@
         <f t="shared" si="4"/>
         <v>0.45929687499999999</v>
       </c>
-      <c r="R29" s="87"/>
+      <c r="R29" s="112"/>
       <c r="S29" s="45" t="s">
         <v>52</v>
       </c>
@@ -9990,8 +10341,8 @@
         <v>7.7805600000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B30" s="87"/>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B30" s="112"/>
       <c r="C30" s="45" t="s">
         <v>51</v>
       </c>
@@ -10039,7 +10390,7 @@
         <f t="shared" si="4"/>
         <v>0.50226562500000005</v>
       </c>
-      <c r="R30" s="87"/>
+      <c r="R30" s="112"/>
       <c r="S30" s="45" t="s">
         <v>51</v>
       </c>
@@ -10078,140 +10429,128 @@
         <v>7.8400400000000009E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" s="87"/>
-      <c r="C31" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="112"/>
+      <c r="C31" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="107">
-        <f t="shared" ref="D31" si="6">1-(0/1280)</f>
-        <v>1</v>
-      </c>
-      <c r="E31" s="107">
-        <f t="shared" ref="E31:M31" si="7">1-(0/1280)</f>
-        <v>1</v>
-      </c>
-      <c r="F31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="H31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="I31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="K31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="L31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="M31" s="107">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="N31" s="107">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="R31" s="87"/>
-      <c r="S31" s="106" t="s">
+      <c r="D31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="K31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="L31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="M31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="N31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="R31" s="112"/>
+      <c r="S31" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="T31" s="108">
-        <v>0</v>
-      </c>
-      <c r="U31" s="108">
-        <v>0</v>
-      </c>
-      <c r="V31" s="108">
-        <v>0</v>
-      </c>
-      <c r="W31" s="108">
-        <v>0</v>
-      </c>
-      <c r="X31" s="108">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="108">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="108">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="108">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="108">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="108">
-        <v>0</v>
-      </c>
-      <c r="AD31" s="108">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="T31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="U31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="V31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="W31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="X31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD31" s="55" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B34" s="88" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="88"/>
-      <c r="D34" s="87" t="s">
+      <c r="B34" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="93"/>
+      <c r="D34" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="87"/>
-      <c r="K34" s="87"/>
-      <c r="L34" s="87"/>
-      <c r="M34" s="87"/>
-      <c r="N34" s="89" t="s">
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="94"/>
+      <c r="I34" s="94"/>
+      <c r="J34" s="94"/>
+      <c r="K34" s="94"/>
+      <c r="L34" s="94"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="R34" s="88" t="s">
-        <v>111</v>
-      </c>
-      <c r="S34" s="88"/>
-      <c r="T34" s="87" t="s">
+      <c r="R34" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="S34" s="93"/>
+      <c r="T34" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="U34" s="87"/>
-      <c r="V34" s="87"/>
-      <c r="W34" s="87"/>
-      <c r="X34" s="87"/>
-      <c r="Y34" s="87"/>
-      <c r="Z34" s="87"/>
-      <c r="AA34" s="87"/>
-      <c r="AB34" s="87"/>
-      <c r="AC34" s="87"/>
-      <c r="AD34" s="89" t="s">
+      <c r="U34" s="94"/>
+      <c r="V34" s="94"/>
+      <c r="W34" s="94"/>
+      <c r="X34" s="94"/>
+      <c r="Y34" s="94"/>
+      <c r="Z34" s="94"/>
+      <c r="AA34" s="94"/>
+      <c r="AB34" s="94"/>
+      <c r="AC34" s="94"/>
+      <c r="AD34" s="90" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B35" s="88"/>
-      <c r="C35" s="88"/>
+    <row r="35" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="93"/>
+      <c r="C35" s="93"/>
       <c r="D35" s="45">
         <v>1</v>
       </c>
@@ -10242,9 +10581,9 @@
       <c r="M35" s="45">
         <v>10</v>
       </c>
-      <c r="N35" s="89"/>
-      <c r="R35" s="88"/>
-      <c r="S35" s="88"/>
+      <c r="N35" s="90"/>
+      <c r="R35" s="93"/>
+      <c r="S35" s="93"/>
       <c r="T35" s="45">
         <v>1</v>
       </c>
@@ -10275,11 +10614,11 @@
       <c r="AC35" s="45">
         <v>10</v>
       </c>
-      <c r="AD35" s="89"/>
+      <c r="AD35" s="90"/>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B36" s="87" t="s">
-        <v>107</v>
+      <c r="B36" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="C36" s="45" t="s">
         <v>1</v>
@@ -10328,8 +10667,8 @@
         <f>AVERAGE(D36:M36)</f>
         <v>0.10200743494423789</v>
       </c>
-      <c r="R36" s="87" t="s">
-        <v>108</v>
+      <c r="R36" s="112" t="s">
+        <v>110</v>
       </c>
       <c r="S36" s="45" t="s">
         <v>1</v>
@@ -10370,7 +10709,7 @@
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B37" s="87"/>
+      <c r="B37" s="112"/>
       <c r="C37" s="45" t="s">
         <v>2</v>
       </c>
@@ -10415,10 +10754,10 @@
         <v>0.28996282527881045</v>
       </c>
       <c r="N37" s="50">
-        <f t="shared" ref="N37:N41" si="8">AVERAGE(D37:M37)</f>
+        <f t="shared" ref="N37:N41" si="6">AVERAGE(D37:M37)</f>
         <v>0.16988847583643124</v>
       </c>
-      <c r="R37" s="87"/>
+      <c r="R37" s="112"/>
       <c r="S37" s="45" t="s">
         <v>2</v>
       </c>
@@ -10453,12 +10792,12 @@
         <v>0.10981200000000001</v>
       </c>
       <c r="AD37" s="52">
-        <f t="shared" ref="AD37:AD41" si="9">AVERAGE(T37:AC37)</f>
+        <f t="shared" ref="AD37:AD41" si="7">AVERAGE(T37:AC37)</f>
         <v>0.11642079999999999</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B38" s="87"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="45" t="s">
         <v>3</v>
       </c>
@@ -10503,10 +10842,10 @@
         <v>0.3197026022304833</v>
       </c>
       <c r="N38" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.37724907063197022</v>
       </c>
-      <c r="R38" s="87"/>
+      <c r="R38" s="112"/>
       <c r="S38" s="45" t="s">
         <v>3</v>
       </c>
@@ -10541,12 +10880,12 @@
         <v>0.10173599999999999</v>
       </c>
       <c r="AD38" s="52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9.1741199999999995E-2</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B39" s="87"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="45" t="s">
         <v>52</v>
       </c>
@@ -10591,10 +10930,10 @@
         <v>0.34795539033457246</v>
       </c>
       <c r="N39" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.45933085501858739</v>
       </c>
-      <c r="R39" s="87"/>
+      <c r="R39" s="112"/>
       <c r="S39" s="45" t="s">
         <v>52</v>
       </c>
@@ -10629,12 +10968,12 @@
         <v>9.6271999999999996E-2</v>
       </c>
       <c r="AD39" s="52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8.16828E-2</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B40" s="87"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="45" t="s">
         <v>51</v>
       </c>
@@ -10679,10 +11018,10 @@
         <v>0.31226765799256506</v>
       </c>
       <c r="N40" s="50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.54542750929368033</v>
       </c>
-      <c r="R40" s="87"/>
+      <c r="R40" s="112"/>
       <c r="S40" s="45" t="s">
         <v>51</v>
       </c>
@@ -10717,119 +11056,97 @@
         <v>0.10668800000000001</v>
       </c>
       <c r="AD40" s="52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8.2377599999999995E-2</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="87"/>
-      <c r="C41" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="112"/>
+      <c r="C41" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="107">
-        <f t="shared" ref="D37:D41" si="10">1-(0/1345)</f>
-        <v>1</v>
-      </c>
-      <c r="E41" s="107">
-        <f t="shared" ref="E36:M41" si="11">1-(0/1345)</f>
-        <v>1</v>
-      </c>
-      <c r="F41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="G41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="H41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="I41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="J41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="K41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="L41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="M41" s="107">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="N41" s="107">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="R41" s="87"/>
-      <c r="S41" s="106" t="s">
+      <c r="D41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="I41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="J41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="K41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="L41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="M41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="N41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="R41" s="112"/>
+      <c r="S41" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="T41" s="108">
-        <v>0</v>
-      </c>
-      <c r="U41" s="108">
-        <v>0</v>
-      </c>
-      <c r="V41" s="108">
-        <v>0</v>
-      </c>
-      <c r="W41" s="108">
-        <v>0</v>
-      </c>
-      <c r="X41" s="108">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="108">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="108">
-        <v>0</v>
-      </c>
-      <c r="AA41" s="108">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="108">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="108">
-        <v>0</v>
-      </c>
-      <c r="AD41" s="108">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="T41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="U41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="V41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="W41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="X41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD41" s="55" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="R4:S5"/>
-    <mergeCell ref="T4:AC4"/>
-    <mergeCell ref="AD4:AD5"/>
-    <mergeCell ref="R6:R11"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="D14:M14"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:M4"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:M34"/>
-    <mergeCell ref="N34:N35"/>
+  <mergeCells count="38">
+    <mergeCell ref="AG4:AG5"/>
+    <mergeCell ref="AH4:AH5"/>
+    <mergeCell ref="AI4:AN4"/>
+    <mergeCell ref="AG14:AG15"/>
+    <mergeCell ref="AH14:AH15"/>
+    <mergeCell ref="AI14:AN14"/>
     <mergeCell ref="T34:AC34"/>
     <mergeCell ref="AD34:AD35"/>
     <mergeCell ref="R36:R41"/>
@@ -10846,6 +11163,22 @@
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="B24:C25"/>
     <mergeCell ref="D24:M24"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:M34"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="R4:S5"/>
+    <mergeCell ref="T4:AC4"/>
+    <mergeCell ref="AD4:AD5"/>
+    <mergeCell ref="R6:R11"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:M14"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:M4"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -10929,7 +11262,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="102">
+      <c r="B8" s="97">
         <v>584</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -10950,7 +11283,7 @@
       <c r="H8" s="1">
         <v>8.0800000000000004E-3</v>
       </c>
-      <c r="L8" s="92">
+      <c r="L8" s="98">
         <v>584</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -10973,7 +11306,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="102"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="1" t="s">
         <v>68</v>
       </c>
@@ -10992,7 +11325,7 @@
       <c r="H9" s="1">
         <v>4.5935999999999998E-2</v>
       </c>
-      <c r="L9" s="93"/>
+      <c r="L9" s="99"/>
       <c r="M9" s="1" t="s">
         <v>65</v>
       </c>
@@ -11018,7 +11351,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="103">
+      <c r="B10" s="95">
         <v>980</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -11039,7 +11372,7 @@
       <c r="H10" s="16">
         <v>1.2456E-2</v>
       </c>
-      <c r="L10" s="93"/>
+      <c r="L10" s="99"/>
       <c r="M10" s="1" t="s">
         <v>61</v>
       </c>
@@ -11060,7 +11393,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="103"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="16" t="s">
         <v>68</v>
       </c>
@@ -11079,7 +11412,7 @@
       <c r="H11" s="16">
         <v>6.3119999999999996E-2</v>
       </c>
-      <c r="L11" s="94"/>
+      <c r="L11" s="100"/>
       <c r="M11" s="1" t="s">
         <v>66</v>
       </c>
@@ -11105,7 +11438,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="87">
+      <c r="B12" s="94">
         <v>1280</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -11126,7 +11459,7 @@
       <c r="H12" s="4">
         <v>1.5299999999999999E-2</v>
       </c>
-      <c r="L12" s="95">
+      <c r="L12" s="101">
         <v>980</v>
       </c>
       <c r="M12" s="16" t="s">
@@ -11149,7 +11482,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="87"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="4" t="s">
         <v>68</v>
       </c>
@@ -11168,7 +11501,7 @@
       <c r="H13" s="4">
         <v>6.6844000000000001E-2</v>
       </c>
-      <c r="L13" s="96"/>
+      <c r="L13" s="102"/>
       <c r="M13" s="16" t="s">
         <v>66</v>
       </c>
@@ -11194,7 +11527,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="101">
+      <c r="B14" s="96">
         <v>1345</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -11215,7 +11548,7 @@
       <c r="H14" s="7">
         <v>1.5807999999999999E-2</v>
       </c>
-      <c r="L14" s="96"/>
+      <c r="L14" s="102"/>
       <c r="M14" s="16" t="s">
         <v>61</v>
       </c>
@@ -11236,7 +11569,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="101"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="7" t="s">
         <v>68</v>
       </c>
@@ -11255,7 +11588,7 @@
       <c r="H15" s="7">
         <v>6.7227999999999996E-2</v>
       </c>
-      <c r="L15" s="97"/>
+      <c r="L15" s="103"/>
       <c r="M15" s="16" t="s">
         <v>66</v>
       </c>
@@ -11281,7 +11614,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L16" s="98">
+      <c r="L16" s="104">
         <v>1280</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -11304,7 +11637,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L17" s="99"/>
+      <c r="L17" s="105"/>
       <c r="M17" s="4" t="s">
         <v>65</v>
       </c>
@@ -11330,7 +11663,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L18" s="99"/>
+      <c r="L18" s="105"/>
       <c r="M18" s="4" t="s">
         <v>61</v>
       </c>
@@ -11351,7 +11684,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L19" s="100"/>
+      <c r="L19" s="106"/>
       <c r="M19" s="4" t="s">
         <v>65</v>
       </c>
@@ -11377,7 +11710,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L20" s="101">
+      <c r="L20" s="96">
         <v>1345</v>
       </c>
       <c r="M20" s="7" t="s">
@@ -11400,7 +11733,7 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L21" s="101"/>
+      <c r="L21" s="96"/>
       <c r="M21" s="7" t="s">
         <v>65</v>
       </c>
@@ -11426,7 +11759,7 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L22" s="101"/>
+      <c r="L22" s="96"/>
       <c r="M22" s="7" t="s">
         <v>61</v>
       </c>
@@ -11447,7 +11780,7 @@
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L23" s="101"/>
+      <c r="L23" s="96"/>
       <c r="M23" s="7" t="s">
         <v>65</v>
       </c>
@@ -11501,7 +11834,7 @@
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="102">
+      <c r="B31" s="97">
         <v>584</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -11524,7 +11857,7 @@
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="102"/>
+      <c r="B32" s="97"/>
       <c r="C32" s="1" t="s">
         <v>68</v>
       </c>
@@ -11545,7 +11878,7 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="103">
+      <c r="B33" s="95">
         <v>980</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -11568,7 +11901,7 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="103"/>
+      <c r="B34" s="95"/>
       <c r="C34" s="16" t="s">
         <v>68</v>
       </c>
@@ -11589,7 +11922,7 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="87">
+      <c r="B35" s="94">
         <v>1280</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -11612,7 +11945,7 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="87"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="4" t="s">
         <v>68</v>
       </c>
@@ -11633,7 +11966,7 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="101">
+      <c r="B37" s="96">
         <v>1345</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -11656,7 +11989,7 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="101"/>
+      <c r="B38" s="96"/>
       <c r="C38" s="7" t="s">
         <v>68</v>
       </c>
@@ -11678,6 +12011,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -11685,11 +12023,6 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11715,7 +12048,7 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="107" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -11741,7 +12074,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="104"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="33">
         <v>584</v>
       </c>
@@ -11765,7 +12098,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="33">
         <v>980</v>
       </c>
@@ -11789,7 +12122,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="33">
         <v>1280</v>
       </c>
@@ -11813,7 +12146,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="104"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="33">
         <v>1435</v>
       </c>
@@ -11837,7 +12170,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="104"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="33">
         <v>1640</v>
       </c>
@@ -11861,7 +12194,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="107" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -11887,7 +12220,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
+      <c r="A15" s="107"/>
       <c r="B15" s="33">
         <v>584</v>
       </c>
@@ -11899,7 +12232,7 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
+      <c r="A16" s="107"/>
       <c r="B16" s="33">
         <v>980</v>
       </c>
@@ -11909,11 +12242,11 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="5"/>
-      <c r="K16" s="105" t="s">
+      <c r="K16" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="108"/>
       <c r="P16" s="11" t="s">
         <v>80</v>
       </c>
@@ -11925,7 +12258,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="104"/>
+      <c r="A17" s="107"/>
       <c r="B17" s="33">
         <v>1280</v>
       </c>
@@ -11955,7 +12288,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="104"/>
+      <c r="A18" s="107"/>
       <c r="B18" s="33">
         <v>1435</v>
       </c>
@@ -11985,7 +12318,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="104"/>
+      <c r="A19" s="107"/>
       <c r="B19" s="33">
         <v>1640</v>
       </c>

</xml_diff>

<commit_message>
update hasil uji coba waktu dekompress
</commit_message>
<xml_diff>
--- a/Data Hasil Uji Coba/Uji Coba.xlsx
+++ b/Data Hasil Uji Coba/Uji Coba.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{40882DD1-D8C2-482D-9238-9700EF588061}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Static Buffer" sheetId="1" r:id="rId1"/>
     <sheet name="Dinamic Buffer" sheetId="2" r:id="rId2"/>
     <sheet name="Akurasi Pengiriman" sheetId="5" r:id="rId3"/>
     <sheet name="Efektifitas" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId6"/>
+    <sheet name="Waktu" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="125">
   <si>
     <t>0 x</t>
   </si>
@@ -406,11 +408,23 @@
   <si>
     <t>Waktu Kompresi Pada Panjang Data 1345</t>
   </si>
+  <si>
+    <t>Waktu Dekompresi Pada Panjang Data 584</t>
+  </si>
+  <si>
+    <t>Waktu Dekompresi Pada Panjang Data 980</t>
+  </si>
+  <si>
+    <t>Waktu Dekompresi Pada Panjang Data 1280</t>
+  </si>
+  <si>
+    <t>Waktu Dekompresi Pada Panjang Data 1345</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -714,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -839,6 +853,21 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -956,6 +985,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -997,18 +1029,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2090,7 +2110,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2370,7 +2396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R52"/>
   <sheetViews>
     <sheetView topLeftCell="I26" workbookViewId="0">
@@ -2402,32 +2428,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="K2" s="83" t="s">
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="K2" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
     </row>
     <row r="3" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="82"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
         <v>1</v>
@@ -2444,10 +2470,10 @@
       <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="81" t="s">
+      <c r="K3" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="82"/>
+      <c r="L3" s="87"/>
       <c r="M3" s="14"/>
       <c r="N3" s="15" t="s">
         <v>1</v>
@@ -2466,10 +2492,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="63">
+      <c r="A4" s="68">
         <v>584</v>
       </c>
-      <c r="B4" s="64"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -2488,10 +2514,10 @@
       <c r="H4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="63">
+      <c r="K4" s="68">
         <v>584</v>
       </c>
-      <c r="L4" s="64"/>
+      <c r="L4" s="69"/>
       <c r="M4" s="1" t="s">
         <v>30</v>
       </c>
@@ -2512,8 +2538,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -2532,8 +2558,8 @@
       <c r="H5" s="1">
         <v>21</v>
       </c>
-      <c r="K5" s="65"/>
-      <c r="L5" s="66"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="71"/>
       <c r="M5" s="1" t="s">
         <v>21</v>
       </c>
@@ -2554,8 +2580,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2579,8 +2605,8 @@
         <f>($A$4-H5)/$A$4</f>
         <v>0.96404109589041098</v>
       </c>
-      <c r="K6" s="65"/>
-      <c r="L6" s="66"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="71"/>
       <c r="M6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2606,8 +2632,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2626,8 +2652,8 @@
       <c r="H7" s="1">
         <v>427</v>
       </c>
-      <c r="K7" s="65"/>
-      <c r="L7" s="66"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="71"/>
       <c r="M7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2648,8 +2674,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
-      <c r="B8" s="68"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
@@ -2673,8 +2699,8 @@
         <f>($A$4-H7)/$A$4</f>
         <v>0.26883561643835618</v>
       </c>
-      <c r="K8" s="67"/>
-      <c r="L8" s="68"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="73"/>
       <c r="M8" s="1" t="s">
         <v>34</v>
       </c>
@@ -2700,10 +2726,10 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="69">
+      <c r="A9" s="74">
         <v>980</v>
       </c>
-      <c r="B9" s="70"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="16" t="s">
         <v>30</v>
       </c>
@@ -2722,10 +2748,10 @@
       <c r="H9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="69">
+      <c r="K9" s="74">
         <v>980</v>
       </c>
-      <c r="L9" s="70"/>
+      <c r="L9" s="75"/>
       <c r="M9" s="16" t="s">
         <v>30</v>
       </c>
@@ -2746,8 +2772,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="16" t="s">
         <v>21</v>
       </c>
@@ -2766,8 +2792,8 @@
       <c r="H10" s="16">
         <v>33</v>
       </c>
-      <c r="K10" s="71"/>
-      <c r="L10" s="72"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="77"/>
       <c r="M10" s="16" t="s">
         <v>21</v>
       </c>
@@ -2788,8 +2814,8 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
@@ -2813,8 +2839,8 @@
         <f>($A$9-H10)/$A$9</f>
         <v>0.96632653061224494</v>
       </c>
-      <c r="K11" s="71"/>
-      <c r="L11" s="72"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="77"/>
       <c r="M11" s="16" t="s">
         <v>35</v>
       </c>
@@ -2840,8 +2866,8 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="16" t="s">
         <v>22</v>
       </c>
@@ -2860,8 +2886,8 @@
       <c r="H12" s="16">
         <v>564</v>
       </c>
-      <c r="K12" s="71"/>
-      <c r="L12" s="72"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="77"/>
       <c r="M12" s="16" t="s">
         <v>22</v>
       </c>
@@ -2882,8 +2908,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="74"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="16" t="s">
         <v>34</v>
       </c>
@@ -2907,8 +2933,8 @@
         <f>($A$9-H12)/$A$9</f>
         <v>0.42448979591836733</v>
       </c>
-      <c r="K13" s="73"/>
-      <c r="L13" s="74"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="79"/>
       <c r="M13" s="16" t="s">
         <v>34</v>
       </c>
@@ -2934,10 +2960,10 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="75">
+      <c r="A14" s="80">
         <v>1280</v>
       </c>
-      <c r="B14" s="76"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
@@ -2956,10 +2982,10 @@
       <c r="H14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="75">
+      <c r="K14" s="80">
         <v>1280</v>
       </c>
-      <c r="L14" s="76"/>
+      <c r="L14" s="81"/>
       <c r="M14" s="13" t="s">
         <v>30</v>
       </c>
@@ -2980,8 +3006,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="77"/>
-      <c r="B15" s="78"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
@@ -2998,8 +3024,8 @@
         <v>68</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="78"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="83"/>
       <c r="M15" s="4" t="s">
         <v>21</v>
       </c>
@@ -3020,8 +3046,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
-      <c r="B16" s="78"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
@@ -3045,8 +3071,8 @@
         <f>($A$14-H15)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K16" s="77"/>
-      <c r="L16" s="78"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="83"/>
       <c r="M16" s="4" t="s">
         <v>35</v>
       </c>
@@ -3072,8 +3098,8 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
-      <c r="B17" s="78"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3090,8 +3116,8 @@
         <v>1120</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="K17" s="77"/>
-      <c r="L17" s="78"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="83"/>
       <c r="M17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3112,8 +3138,8 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
-      <c r="B18" s="80"/>
+      <c r="A18" s="84"/>
+      <c r="B18" s="85"/>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
@@ -3137,8 +3163,8 @@
         <f>($A$14-H17)/$A$14</f>
         <v>1</v>
       </c>
-      <c r="K18" s="79"/>
-      <c r="L18" s="80"/>
+      <c r="K18" s="84"/>
+      <c r="L18" s="85"/>
       <c r="M18" s="4" t="s">
         <v>34</v>
       </c>
@@ -3164,10 +3190,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="56">
+      <c r="A19" s="61">
         <v>1345</v>
       </c>
-      <c r="B19" s="57"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
@@ -3186,10 +3212,10 @@
       <c r="H19" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K19" s="56">
+      <c r="K19" s="61">
         <v>1345</v>
       </c>
-      <c r="L19" s="57"/>
+      <c r="L19" s="62"/>
       <c r="M19" s="7" t="s">
         <v>30</v>
       </c>
@@ -3210,8 +3236,8 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
@@ -3228,8 +3254,8 @@
         <v>129</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="59"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="64"/>
       <c r="M20" s="7" t="s">
         <v>21</v>
       </c>
@@ -3250,8 +3276,8 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="59"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="7" t="s">
         <v>35</v>
       </c>
@@ -3272,8 +3298,8 @@
         <v>0.90408921933085507</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="59"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="64"/>
       <c r="M21" s="7" t="s">
         <v>35</v>
       </c>
@@ -3299,8 +3325,8 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
-      <c r="B22" s="59"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="64"/>
       <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
@@ -3317,8 +3343,8 @@
         <v>1182</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="59"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="64"/>
       <c r="M22" s="7" t="s">
         <v>22</v>
       </c>
@@ -3337,8 +3363,8 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="60"/>
-      <c r="B23" s="61"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="7" t="s">
         <v>34</v>
       </c>
@@ -3359,8 +3385,8 @@
         <v>0.12118959107806691</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="61"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="66"/>
       <c r="M23" s="7" t="s">
         <v>34</v>
       </c>
@@ -3383,10 +3409,10 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K24" s="62">
+      <c r="K24" s="67">
         <v>1640</v>
       </c>
-      <c r="L24" s="62"/>
+      <c r="L24" s="67"/>
       <c r="M24" s="24" t="s">
         <v>30</v>
       </c>
@@ -3407,10 +3433,10 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="82"/>
+      <c r="B28" s="87"/>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
         <v>1</v>
@@ -3427,10 +3453,10 @@
       <c r="H28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="81" t="s">
+      <c r="K28" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="L28" s="82"/>
+      <c r="L28" s="87"/>
       <c r="M28" s="14"/>
       <c r="N28" s="15" t="s">
         <v>1</v>
@@ -3449,10 +3475,10 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="63">
+      <c r="A29" s="68">
         <v>584</v>
       </c>
-      <c r="B29" s="64"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
@@ -3472,10 +3498,10 @@
         <v>8.1119999999999994E-3</v>
       </c>
       <c r="J29" s="24"/>
-      <c r="K29" s="63">
+      <c r="K29" s="68">
         <v>584</v>
       </c>
-      <c r="L29" s="64"/>
+      <c r="L29" s="69"/>
       <c r="M29" s="1" t="s">
         <v>23</v>
       </c>
@@ -3496,8 +3522,8 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="65"/>
-      <c r="B30" s="66"/>
+      <c r="A30" s="70"/>
+      <c r="B30" s="71"/>
       <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
@@ -3516,8 +3542,8 @@
       <c r="H30" s="1">
         <v>3.248E-3</v>
       </c>
-      <c r="K30" s="65"/>
-      <c r="L30" s="66"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="71"/>
       <c r="M30" s="1" t="s">
         <v>24</v>
       </c>
@@ -3538,8 +3564,8 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="65"/>
-      <c r="B31" s="66"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="71"/>
       <c r="C31" s="19" t="s">
         <v>32</v>
       </c>
@@ -3563,8 +3589,8 @@
         <f t="shared" si="0"/>
         <v>1.1359999999999999E-2</v>
       </c>
-      <c r="K31" s="65"/>
-      <c r="L31" s="66"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="71"/>
       <c r="M31" s="19" t="s">
         <v>32</v>
       </c>
@@ -3590,8 +3616,8 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="65"/>
-      <c r="B32" s="66"/>
+      <c r="A32" s="70"/>
+      <c r="B32" s="71"/>
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3611,8 +3637,8 @@
         <v>4.0691999999999999E-2</v>
       </c>
       <c r="J32" s="24"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="66"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="71"/>
       <c r="M32" s="1" t="s">
         <v>25</v>
       </c>
@@ -3633,8 +3659,8 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="65"/>
-      <c r="B33" s="66"/>
+      <c r="A33" s="70"/>
+      <c r="B33" s="71"/>
       <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3653,8 +3679,8 @@
       <c r="H33" s="1">
         <v>1.7328E-2</v>
       </c>
-      <c r="K33" s="65"/>
-      <c r="L33" s="66"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="71"/>
       <c r="M33" s="1" t="s">
         <v>26</v>
       </c>
@@ -3675,8 +3701,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="67"/>
-      <c r="B34" s="68"/>
+      <c r="A34" s="72"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="19" t="s">
         <v>32</v>
       </c>
@@ -3700,8 +3726,8 @@
         <f t="shared" si="2"/>
         <v>5.8020000000000002E-2</v>
       </c>
-      <c r="K34" s="67"/>
-      <c r="L34" s="68"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="73"/>
       <c r="M34" s="19" t="s">
         <v>32</v>
       </c>
@@ -3727,10 +3753,10 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="69">
+      <c r="A35" s="74">
         <v>980</v>
       </c>
-      <c r="B35" s="70"/>
+      <c r="B35" s="75"/>
       <c r="C35" s="16" t="s">
         <v>23</v>
       </c>
@@ -3750,10 +3776,10 @@
         <v>1.2716E-2</v>
       </c>
       <c r="J35" s="24"/>
-      <c r="K35" s="69">
+      <c r="K35" s="74">
         <v>980</v>
       </c>
-      <c r="L35" s="70"/>
+      <c r="L35" s="75"/>
       <c r="M35" s="16" t="s">
         <v>23</v>
       </c>
@@ -3774,8 +3800,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
-      <c r="B36" s="72"/>
+      <c r="A36" s="76"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="16" t="s">
         <v>24</v>
       </c>
@@ -3794,8 +3820,8 @@
       <c r="H36" s="16">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="K36" s="71"/>
-      <c r="L36" s="72"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="77"/>
       <c r="M36" s="16" t="s">
         <v>24</v>
       </c>
@@ -3816,8 +3842,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
-      <c r="B37" s="72"/>
+      <c r="A37" s="76"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="19" t="s">
         <v>32</v>
       </c>
@@ -3841,8 +3867,8 @@
         <f t="shared" si="4"/>
         <v>1.7916000000000001E-2</v>
       </c>
-      <c r="K37" s="71"/>
-      <c r="L37" s="72"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="77"/>
       <c r="M37" s="19" t="s">
         <v>32</v>
       </c>
@@ -3868,8 +3894,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="71"/>
-      <c r="B38" s="72"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -3889,8 +3915,8 @@
         <v>5.5975999999999998E-2</v>
       </c>
       <c r="J38" s="24"/>
-      <c r="K38" s="71"/>
-      <c r="L38" s="72"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="77"/>
       <c r="M38" s="16" t="s">
         <v>25</v>
       </c>
@@ -3911,8 +3937,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
-      <c r="B39" s="72"/>
+      <c r="A39" s="76"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="16" t="s">
         <v>26</v>
       </c>
@@ -3931,8 +3957,8 @@
       <c r="H39" s="16">
         <v>2.3768000000000001E-2</v>
       </c>
-      <c r="K39" s="71"/>
-      <c r="L39" s="72"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="77"/>
       <c r="M39" s="16" t="s">
         <v>26</v>
       </c>
@@ -3953,8 +3979,8 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="73"/>
-      <c r="B40" s="74"/>
+      <c r="A40" s="78"/>
+      <c r="B40" s="79"/>
       <c r="C40" s="19" t="s">
         <v>32</v>
       </c>
@@ -3978,8 +4004,8 @@
         <f t="shared" si="6"/>
         <v>7.9743999999999995E-2</v>
       </c>
-      <c r="K40" s="73"/>
-      <c r="L40" s="74"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="79"/>
       <c r="M40" s="19" t="s">
         <v>32</v>
       </c>
@@ -4005,10 +4031,10 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="75">
+      <c r="A41" s="80">
         <v>1280</v>
       </c>
-      <c r="B41" s="76"/>
+      <c r="B41" s="81"/>
       <c r="C41" s="4" t="s">
         <v>23</v>
       </c>
@@ -4026,10 +4052,10 @@
       </c>
       <c r="H41" s="5"/>
       <c r="J41" s="24"/>
-      <c r="K41" s="75">
+      <c r="K41" s="80">
         <v>1280</v>
       </c>
-      <c r="L41" s="76"/>
+      <c r="L41" s="81"/>
       <c r="M41" s="4" t="s">
         <v>23</v>
       </c>
@@ -4050,8 +4076,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="77"/>
-      <c r="B42" s="78"/>
+      <c r="A42" s="82"/>
+      <c r="B42" s="83"/>
       <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
@@ -4068,8 +4094,8 @@
         <v>9.476E-3</v>
       </c>
       <c r="H42" s="5"/>
-      <c r="K42" s="77"/>
-      <c r="L42" s="78"/>
+      <c r="K42" s="82"/>
+      <c r="L42" s="83"/>
       <c r="M42" s="4" t="s">
         <v>24</v>
       </c>
@@ -4090,8 +4116,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="77"/>
-      <c r="B43" s="78"/>
+      <c r="A43" s="82"/>
+      <c r="B43" s="83"/>
       <c r="C43" s="19" t="s">
         <v>32</v>
       </c>
@@ -4112,8 +4138,8 @@
         <v>2.7875999999999998E-2</v>
       </c>
       <c r="H43" s="5"/>
-      <c r="K43" s="77"/>
-      <c r="L43" s="78"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="83"/>
       <c r="M43" s="19" t="s">
         <v>32</v>
       </c>
@@ -4139,8 +4165,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="77"/>
-      <c r="B44" s="78"/>
+      <c r="A44" s="82"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
@@ -4158,8 +4184,8 @@
       </c>
       <c r="H44" s="5"/>
       <c r="J44" s="24"/>
-      <c r="K44" s="77"/>
-      <c r="L44" s="78"/>
+      <c r="K44" s="82"/>
+      <c r="L44" s="83"/>
       <c r="M44" s="4" t="s">
         <v>25</v>
       </c>
@@ -4180,8 +4206,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="77"/>
-      <c r="B45" s="78"/>
+      <c r="A45" s="82"/>
+      <c r="B45" s="83"/>
       <c r="C45" s="4" t="s">
         <v>26</v>
       </c>
@@ -4198,8 +4224,8 @@
         <v>4.3580000000000001E-2</v>
       </c>
       <c r="H45" s="5"/>
-      <c r="K45" s="77"/>
-      <c r="L45" s="78"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="83"/>
       <c r="M45" s="4" t="s">
         <v>26</v>
       </c>
@@ -4220,8 +4246,8 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="79"/>
-      <c r="B46" s="80"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="85"/>
       <c r="C46" s="19" t="s">
         <v>32</v>
       </c>
@@ -4242,8 +4268,8 @@
         <v>0.146428</v>
       </c>
       <c r="H46" s="5"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="80"/>
+      <c r="K46" s="84"/>
+      <c r="L46" s="85"/>
       <c r="M46" s="19" t="s">
         <v>32</v>
       </c>
@@ -4269,10 +4295,10 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="56">
+      <c r="A47" s="61">
         <v>1345</v>
       </c>
-      <c r="B47" s="57"/>
+      <c r="B47" s="62"/>
       <c r="C47" s="7" t="s">
         <v>23</v>
       </c>
@@ -4290,10 +4316,10 @@
       </c>
       <c r="H47" s="5"/>
       <c r="J47" s="24"/>
-      <c r="K47" s="56">
+      <c r="K47" s="61">
         <v>1345</v>
       </c>
-      <c r="L47" s="57"/>
+      <c r="L47" s="62"/>
       <c r="M47" s="7" t="s">
         <v>23</v>
       </c>
@@ -4314,8 +4340,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="58"/>
-      <c r="B48" s="59"/>
+      <c r="A48" s="63"/>
+      <c r="B48" s="64"/>
       <c r="C48" s="7" t="s">
         <v>24</v>
       </c>
@@ -4332,8 +4358,8 @@
         <v>9.9319999999999999E-3</v>
       </c>
       <c r="H48" s="5"/>
-      <c r="K48" s="58"/>
-      <c r="L48" s="59"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="64"/>
       <c r="M48" s="7" t="s">
         <v>24</v>
       </c>
@@ -4352,8 +4378,8 @@
       <c r="R48" s="5"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="58"/>
-      <c r="B49" s="59"/>
+      <c r="A49" s="63"/>
+      <c r="B49" s="64"/>
       <c r="C49" s="19" t="s">
         <v>32</v>
       </c>
@@ -4374,8 +4400,8 @@
         <v>2.8931999999999999E-2</v>
       </c>
       <c r="H49" s="5"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="59"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="64"/>
       <c r="M49" s="19" t="s">
         <v>32</v>
       </c>
@@ -4398,8 +4424,8 @@
       <c r="R49" s="5"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="58"/>
-      <c r="B50" s="59"/>
+      <c r="A50" s="63"/>
+      <c r="B50" s="64"/>
       <c r="C50" s="7" t="s">
         <v>25</v>
       </c>
@@ -4417,8 +4443,8 @@
       </c>
       <c r="H50" s="5"/>
       <c r="J50" s="24"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="59"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="64"/>
       <c r="M50" s="7" t="s">
         <v>25</v>
       </c>
@@ -4437,8 +4463,8 @@
       <c r="R50" s="5"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="58"/>
-      <c r="B51" s="59"/>
+      <c r="A51" s="63"/>
+      <c r="B51" s="64"/>
       <c r="C51" s="7" t="s">
         <v>26</v>
       </c>
@@ -4455,8 +4481,8 @@
         <v>4.5887999999999998E-2</v>
       </c>
       <c r="H51" s="5"/>
-      <c r="K51" s="58"/>
-      <c r="L51" s="59"/>
+      <c r="K51" s="63"/>
+      <c r="L51" s="64"/>
       <c r="M51" s="7" t="s">
         <v>26</v>
       </c>
@@ -4475,8 +4501,8 @@
       <c r="R51" s="5"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="60"/>
-      <c r="B52" s="61"/>
+      <c r="A52" s="65"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="19" t="s">
         <v>32</v>
       </c>
@@ -4497,8 +4523,8 @@
         <v>0.15465999999999999</v>
       </c>
       <c r="H52" s="5"/>
-      <c r="K52" s="60"/>
-      <c r="L52" s="61"/>
+      <c r="K52" s="65"/>
+      <c r="L52" s="66"/>
       <c r="M52" s="19" t="s">
         <v>32</v>
       </c>
@@ -4552,7 +4578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -4582,32 +4608,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="87"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15" t="s">
         <v>1</v>
@@ -4659,10 +4685,10 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="63">
+      <c r="A3" s="68">
         <v>584</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -4716,8 +4742,8 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
@@ -4771,8 +4797,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
@@ -4842,8 +4868,8 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4897,8 +4923,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
-      <c r="B7" s="68"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="73"/>
       <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
@@ -4968,10 +4994,10 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="69">
+      <c r="A8" s="74">
         <v>980</v>
       </c>
-      <c r="B8" s="70"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="16" t="s">
         <v>30</v>
       </c>
@@ -5022,8 +5048,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
@@ -5077,8 +5103,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="16" t="s">
         <v>35</v>
       </c>
@@ -5144,8 +5170,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="16" t="s">
         <v>22</v>
       </c>
@@ -5199,8 +5225,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="74"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="16" t="s">
         <v>34</v>
       </c>
@@ -5266,10 +5292,10 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="75">
+      <c r="A13" s="80">
         <v>1280</v>
       </c>
-      <c r="B13" s="76"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
@@ -5320,8 +5346,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
-      <c r="B14" s="78"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
@@ -5375,8 +5401,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="77"/>
-      <c r="B15" s="78"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
@@ -5442,8 +5468,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
-      <c r="B16" s="78"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
@@ -5497,8 +5523,8 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
-      <c r="B17" s="80"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
@@ -5564,10 +5590,10 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="56">
+      <c r="A18" s="61">
         <v>1345</v>
       </c>
-      <c r="B18" s="57"/>
+      <c r="B18" s="62"/>
       <c r="C18" s="7" t="s">
         <v>30</v>
       </c>
@@ -5621,8 +5647,8 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="7" t="s">
         <v>21</v>
       </c>
@@ -5679,8 +5705,8 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="7" t="s">
         <v>35</v>
       </c>
@@ -5746,8 +5772,8 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="59"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
@@ -5801,8 +5827,8 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="60"/>
-      <c r="B22" s="61"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -5868,10 +5894,10 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="84">
+      <c r="A23" s="89">
         <v>1640</v>
       </c>
-      <c r="B23" s="85"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="39" t="s">
         <v>30</v>
       </c>
@@ -5902,8 +5928,8 @@
       <c r="R23" s="40"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
-      <c r="B24" s="87"/>
+      <c r="A24" s="91"/>
+      <c r="B24" s="92"/>
       <c r="C24" s="39" t="s">
         <v>21</v>
       </c>
@@ -5935,8 +5961,8 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="86"/>
-      <c r="B25" s="87"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="92"/>
       <c r="C25" s="39" t="s">
         <v>35</v>
       </c>
@@ -5999,8 +6025,8 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="86"/>
-      <c r="B26" s="87"/>
+      <c r="A26" s="91"/>
+      <c r="B26" s="92"/>
       <c r="C26" s="39" t="s">
         <v>22</v>
       </c>
@@ -6032,8 +6058,8 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
-      <c r="B27" s="89"/>
+      <c r="A27" s="93"/>
+      <c r="B27" s="94"/>
       <c r="C27" s="39" t="s">
         <v>34</v>
       </c>
@@ -6107,10 +6133,10 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="82"/>
+      <c r="B33" s="87"/>
       <c r="C33" s="14"/>
       <c r="D33" s="15" t="s">
         <v>1</v>
@@ -6159,10 +6185,10 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="63">
+      <c r="A34" s="68">
         <v>584</v>
       </c>
-      <c r="B34" s="64"/>
+      <c r="B34" s="69"/>
       <c r="C34" s="1" t="s">
         <v>23</v>
       </c>
@@ -6213,8 +6239,8 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="65"/>
-      <c r="B35" s="66"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="71"/>
       <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
@@ -6265,8 +6291,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
-      <c r="B36" s="66"/>
+      <c r="A36" s="70"/>
+      <c r="B36" s="71"/>
       <c r="C36" s="19" t="s">
         <v>32</v>
       </c>
@@ -6332,8 +6358,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="65"/>
-      <c r="B37" s="66"/>
+      <c r="A37" s="70"/>
+      <c r="B37" s="71"/>
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
@@ -6384,8 +6410,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="65"/>
-      <c r="B38" s="66"/>
+      <c r="A38" s="70"/>
+      <c r="B38" s="71"/>
       <c r="C38" s="1" t="s">
         <v>26</v>
       </c>
@@ -6436,8 +6462,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="67"/>
-      <c r="B39" s="68"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="19" t="s">
         <v>32</v>
       </c>
@@ -6503,10 +6529,10 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="69">
+      <c r="A40" s="74">
         <v>980</v>
       </c>
-      <c r="B40" s="70"/>
+      <c r="B40" s="75"/>
       <c r="C40" s="16" t="s">
         <v>23</v>
       </c>
@@ -6557,8 +6583,8 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="71"/>
-      <c r="B41" s="72"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="16" t="s">
         <v>24</v>
       </c>
@@ -6609,8 +6635,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="71"/>
-      <c r="B42" s="72"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="19" t="s">
         <v>32</v>
       </c>
@@ -6676,8 +6702,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72"/>
+      <c r="A43" s="76"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="16" t="s">
         <v>25</v>
       </c>
@@ -6728,8 +6754,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="71"/>
-      <c r="B44" s="72"/>
+      <c r="A44" s="76"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="16" t="s">
         <v>26</v>
       </c>
@@ -6780,8 +6806,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="73"/>
-      <c r="B45" s="74"/>
+      <c r="A45" s="78"/>
+      <c r="B45" s="79"/>
       <c r="C45" s="19" t="s">
         <v>32</v>
       </c>
@@ -6847,10 +6873,10 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="75">
+      <c r="A46" s="80">
         <v>1280</v>
       </c>
-      <c r="B46" s="76"/>
+      <c r="B46" s="81"/>
       <c r="C46" s="4" t="s">
         <v>23</v>
       </c>
@@ -6901,8 +6927,8 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="77"/>
-      <c r="B47" s="78"/>
+      <c r="A47" s="82"/>
+      <c r="B47" s="83"/>
       <c r="C47" s="4" t="s">
         <v>24</v>
       </c>
@@ -6953,8 +6979,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="77"/>
-      <c r="B48" s="78"/>
+      <c r="A48" s="82"/>
+      <c r="B48" s="83"/>
       <c r="C48" s="19" t="s">
         <v>32</v>
       </c>
@@ -7020,8 +7046,8 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="77"/>
-      <c r="B49" s="78"/>
+      <c r="A49" s="82"/>
+      <c r="B49" s="83"/>
       <c r="C49" s="4" t="s">
         <v>25</v>
       </c>
@@ -7072,8 +7098,8 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="77"/>
-      <c r="B50" s="78"/>
+      <c r="A50" s="82"/>
+      <c r="B50" s="83"/>
       <c r="C50" s="4" t="s">
         <v>26</v>
       </c>
@@ -7124,8 +7150,8 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="79"/>
-      <c r="B51" s="80"/>
+      <c r="A51" s="84"/>
+      <c r="B51" s="85"/>
       <c r="C51" s="19" t="s">
         <v>32</v>
       </c>
@@ -7191,10 +7217,10 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="56">
+      <c r="A52" s="61">
         <v>1345</v>
       </c>
-      <c r="B52" s="57"/>
+      <c r="B52" s="62"/>
       <c r="C52" s="7" t="s">
         <v>23</v>
       </c>
@@ -7245,8 +7271,8 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="58"/>
-      <c r="B53" s="59"/>
+      <c r="A53" s="63"/>
+      <c r="B53" s="64"/>
       <c r="C53" s="7" t="s">
         <v>24</v>
       </c>
@@ -7297,8 +7323,8 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="58"/>
-      <c r="B54" s="59"/>
+      <c r="A54" s="63"/>
+      <c r="B54" s="64"/>
       <c r="C54" s="19" t="s">
         <v>32</v>
       </c>
@@ -7364,8 +7390,8 @@
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="58"/>
-      <c r="B55" s="59"/>
+      <c r="A55" s="63"/>
+      <c r="B55" s="64"/>
       <c r="C55" s="7" t="s">
         <v>25</v>
       </c>
@@ -7416,8 +7442,8 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="58"/>
-      <c r="B56" s="59"/>
+      <c r="A56" s="63"/>
+      <c r="B56" s="64"/>
       <c r="C56" s="7" t="s">
         <v>26</v>
       </c>
@@ -7468,8 +7494,8 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="60"/>
-      <c r="B57" s="61"/>
+      <c r="A57" s="65"/>
+      <c r="B57" s="66"/>
       <c r="C57" s="19" t="s">
         <v>32</v>
       </c>
@@ -7557,7 +7583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C7:O36"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
@@ -7795,29 +7821,29 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="93" t="s">
+      <c r="C15" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="93"/>
-      <c r="E15" s="94" t="s">
+      <c r="D15" s="98"/>
+      <c r="E15" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="94"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="94"/>
-      <c r="O15" s="90" t="s">
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="95" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
       <c r="E16" s="42">
         <v>1</v>
       </c>
@@ -7848,10 +7874,10 @@
       <c r="N16" s="42">
         <v>10</v>
       </c>
-      <c r="O16" s="90"/>
+      <c r="O16" s="95"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="90" t="s">
+      <c r="C17" s="95" t="s">
         <v>96</v>
       </c>
       <c r="D17" s="42" t="s">
@@ -7887,13 +7913,13 @@
       <c r="N17" s="43">
         <v>41</v>
       </c>
-      <c r="O17" s="91">
+      <c r="O17" s="96">
         <f>SUM(E17:N17)/410</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="90"/>
+      <c r="C18" s="95"/>
       <c r="D18" s="42" t="s">
         <v>98</v>
       </c>
@@ -7927,32 +7953,32 @@
       <c r="N18" s="43">
         <v>0</v>
       </c>
-      <c r="O18" s="92"/>
+      <c r="O18" s="97"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="93" t="s">
+      <c r="C21" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="93"/>
-      <c r="E21" s="94" t="s">
+      <c r="D21" s="98"/>
+      <c r="E21" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="94"/>
-      <c r="J21" s="94"/>
-      <c r="K21" s="94"/>
-      <c r="L21" s="94"/>
-      <c r="M21" s="94"/>
-      <c r="N21" s="94"/>
-      <c r="O21" s="90" t="s">
+      <c r="F21" s="99"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="99"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="99"/>
+      <c r="N21" s="99"/>
+      <c r="O21" s="95" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
       <c r="E22" s="42">
         <v>1</v>
       </c>
@@ -7983,10 +8009,10 @@
       <c r="N22" s="42">
         <v>10</v>
       </c>
-      <c r="O22" s="90"/>
+      <c r="O22" s="95"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="90" t="s">
+      <c r="C23" s="95" t="s">
         <v>96</v>
       </c>
       <c r="D23" s="42" t="s">
@@ -8022,13 +8048,13 @@
       <c r="N23" s="35">
         <v>27</v>
       </c>
-      <c r="O23" s="91">
+      <c r="O23" s="96">
         <f>SUM(E23:N23)/410</f>
         <v>0.86829268292682926</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="90"/>
+      <c r="C24" s="95"/>
       <c r="D24" s="42" t="s">
         <v>98</v>
       </c>
@@ -8062,32 +8088,32 @@
       <c r="N24" s="43">
         <v>14</v>
       </c>
-      <c r="O24" s="92"/>
+      <c r="O24" s="97"/>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="93" t="s">
+      <c r="C27" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="93"/>
-      <c r="E27" s="94" t="s">
+      <c r="D27" s="98"/>
+      <c r="E27" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="94"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="94"/>
-      <c r="I27" s="94"/>
-      <c r="J27" s="94"/>
-      <c r="K27" s="94"/>
-      <c r="L27" s="94"/>
-      <c r="M27" s="94"/>
-      <c r="N27" s="94"/>
-      <c r="O27" s="90" t="s">
+      <c r="F27" s="99"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="99"/>
+      <c r="L27" s="99"/>
+      <c r="M27" s="99"/>
+      <c r="N27" s="99"/>
+      <c r="O27" s="95" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="93"/>
-      <c r="D28" s="93"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
       <c r="E28" s="42">
         <v>1</v>
       </c>
@@ -8118,10 +8144,10 @@
       <c r="N28" s="42">
         <v>10</v>
       </c>
-      <c r="O28" s="90"/>
+      <c r="O28" s="95"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="90" t="s">
+      <c r="C29" s="95" t="s">
         <v>96</v>
       </c>
       <c r="D29" s="42" t="s">
@@ -8157,13 +8183,13 @@
       <c r="N29" s="35">
         <v>29</v>
       </c>
-      <c r="O29" s="91">
+      <c r="O29" s="96">
         <f>SUM(E29:N29)/410</f>
         <v>0.69512195121951215</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="90"/>
+      <c r="C30" s="95"/>
       <c r="D30" s="42" t="s">
         <v>98</v>
       </c>
@@ -8197,7 +8223,7 @@
       <c r="N30" s="43">
         <v>12</v>
       </c>
-      <c r="O30" s="92"/>
+      <c r="O30" s="97"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="46"/>
@@ -8269,11 +8295,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A4:AN41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4:AN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8290,62 +8316,62 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="94" t="s">
+      <c r="C4" s="98"/>
+      <c r="D4" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="90" t="s">
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="95" t="s">
         <v>116</v>
       </c>
-      <c r="R4" s="93" t="s">
+      <c r="R4" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="S4" s="93"/>
-      <c r="T4" s="94" t="s">
+      <c r="S4" s="98"/>
+      <c r="T4" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="U4" s="94"/>
-      <c r="V4" s="94"/>
-      <c r="W4" s="94"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="94"/>
-      <c r="AB4" s="94"/>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="90" t="s">
+      <c r="U4" s="99"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="99"/>
+      <c r="X4" s="99"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="99"/>
+      <c r="AB4" s="99"/>
+      <c r="AC4" s="99"/>
+      <c r="AD4" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="AG4" s="90" t="s">
+      <c r="AG4" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="AH4" s="94" t="s">
+      <c r="AH4" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="AI4" s="94" t="s">
+      <c r="AI4" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="AJ4" s="94"/>
-      <c r="AK4" s="94"/>
-      <c r="AL4" s="94"/>
-      <c r="AM4" s="94"/>
-      <c r="AN4" s="94"/>
+      <c r="AJ4" s="99"/>
+      <c r="AK4" s="99"/>
+      <c r="AL4" s="99"/>
+      <c r="AM4" s="99"/>
+      <c r="AN4" s="99"/>
     </row>
     <row r="5" spans="2:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="45">
         <v>1</v>
       </c>
@@ -8376,9 +8402,9 @@
       <c r="M5" s="45">
         <v>10</v>
       </c>
-      <c r="N5" s="90"/>
-      <c r="R5" s="93"/>
-      <c r="S5" s="93"/>
+      <c r="N5" s="95"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="98"/>
       <c r="T5" s="45">
         <v>1</v>
       </c>
@@ -8409,9 +8435,9 @@
       <c r="AC5" s="45">
         <v>10</v>
       </c>
-      <c r="AD5" s="90"/>
-      <c r="AG5" s="90"/>
-      <c r="AH5" s="94"/>
+      <c r="AD5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="99"/>
       <c r="AI5" s="53" t="s">
         <v>1</v>
       </c>
@@ -8432,7 +8458,7 @@
       </c>
     </row>
     <row r="6" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="100" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="45" t="s">
@@ -8482,7 +8508,7 @@
         <f>AVERAGE(D6:M6)</f>
         <v>9.2636986301369864E-2</v>
       </c>
-      <c r="R6" s="112" t="s">
+      <c r="R6" s="100" t="s">
         <v>110</v>
       </c>
       <c r="S6" s="45" t="s">
@@ -8528,33 +8554,33 @@
       <c r="AH6" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="AI6" s="110">
+      <c r="AI6" s="58">
         <f>AD6</f>
         <v>5.8035200000000009E-2</v>
       </c>
-      <c r="AJ6" s="110">
+      <c r="AJ6" s="58">
         <f>AD7</f>
         <v>4.6922399999999996E-2</v>
       </c>
-      <c r="AK6" s="110">
+      <c r="AK6" s="58">
         <f>AD8</f>
         <v>4.1415600000000004E-2</v>
       </c>
-      <c r="AL6" s="110">
+      <c r="AL6" s="58">
         <f>AD9</f>
         <v>3.2311600000000003E-2</v>
       </c>
-      <c r="AM6" s="110">
+      <c r="AM6" s="58">
         <f>AD10</f>
         <v>2.9476800000000004E-2</v>
       </c>
-      <c r="AN6" s="110">
+      <c r="AN6" s="58">
         <f>AD11</f>
         <v>3.0045600000000006E-2</v>
       </c>
     </row>
     <row r="7" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B7" s="112"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="45" t="s">
         <v>2</v>
       </c>
@@ -8602,7 +8628,7 @@
         <f t="shared" ref="N7:N11" si="0">AVERAGE(D7:M7)</f>
         <v>0.2441780821917808</v>
       </c>
-      <c r="R7" s="112"/>
+      <c r="R7" s="100"/>
       <c r="S7" s="45" t="s">
         <v>2</v>
       </c>
@@ -8672,7 +8698,7 @@
       </c>
     </row>
     <row r="8" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B8" s="112"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="45" t="s">
         <v>3</v>
       </c>
@@ -8720,7 +8746,7 @@
         <f t="shared" si="0"/>
         <v>0.31849315068493156</v>
       </c>
-      <c r="R8" s="112"/>
+      <c r="R8" s="100"/>
       <c r="S8" s="45" t="s">
         <v>3</v>
       </c>
@@ -8790,7 +8816,7 @@
       </c>
     </row>
     <row r="9" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B9" s="112"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="45" t="s">
         <v>52</v>
       </c>
@@ -8838,7 +8864,7 @@
         <f t="shared" si="0"/>
         <v>0.49383561643835616</v>
       </c>
-      <c r="R9" s="112"/>
+      <c r="R9" s="100"/>
       <c r="S9" s="45" t="s">
         <v>52</v>
       </c>
@@ -8908,7 +8934,7 @@
       </c>
     </row>
     <row r="10" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B10" s="112"/>
+      <c r="B10" s="100"/>
       <c r="C10" s="45" t="s">
         <v>51</v>
       </c>
@@ -8956,7 +8982,7 @@
         <f t="shared" si="0"/>
         <v>0.59845890410958913</v>
       </c>
-      <c r="R10" s="112"/>
+      <c r="R10" s="100"/>
       <c r="S10" s="45" t="s">
         <v>51</v>
       </c>
@@ -8996,7 +9022,7 @@
       </c>
     </row>
     <row r="11" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B11" s="112"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="45" t="s">
         <v>69</v>
       </c>
@@ -9044,7 +9070,7 @@
         <f t="shared" si="0"/>
         <v>0.56746575342465744</v>
       </c>
-      <c r="R11" s="112"/>
+      <c r="R11" s="100"/>
       <c r="S11" s="45" t="s">
         <v>69</v>
       </c>
@@ -9084,62 +9110,62 @@
       </c>
     </row>
     <row r="14" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="94" t="s">
+      <c r="C14" s="98"/>
+      <c r="D14" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94"/>
-      <c r="M14" s="94"/>
-      <c r="N14" s="90" t="s">
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="R14" s="93" t="s">
+      <c r="R14" s="98" t="s">
         <v>118</v>
       </c>
-      <c r="S14" s="93"/>
-      <c r="T14" s="94" t="s">
+      <c r="S14" s="98"/>
+      <c r="T14" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="U14" s="94"/>
-      <c r="V14" s="94"/>
-      <c r="W14" s="94"/>
-      <c r="X14" s="94"/>
-      <c r="Y14" s="94"/>
-      <c r="Z14" s="94"/>
-      <c r="AA14" s="94"/>
-      <c r="AB14" s="94"/>
-      <c r="AC14" s="94"/>
-      <c r="AD14" s="90" t="s">
+      <c r="U14" s="99"/>
+      <c r="V14" s="99"/>
+      <c r="W14" s="99"/>
+      <c r="X14" s="99"/>
+      <c r="Y14" s="99"/>
+      <c r="Z14" s="99"/>
+      <c r="AA14" s="99"/>
+      <c r="AB14" s="99"/>
+      <c r="AC14" s="99"/>
+      <c r="AD14" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="AG14" s="90" t="s">
+      <c r="AG14" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="AH14" s="94" t="s">
+      <c r="AH14" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="AI14" s="94" t="s">
+      <c r="AI14" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="AJ14" s="94"/>
-      <c r="AK14" s="94"/>
-      <c r="AL14" s="94"/>
-      <c r="AM14" s="94"/>
-      <c r="AN14" s="94"/>
+      <c r="AJ14" s="99"/>
+      <c r="AK14" s="99"/>
+      <c r="AL14" s="99"/>
+      <c r="AM14" s="99"/>
+      <c r="AN14" s="99"/>
     </row>
     <row r="15" spans="2:40" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="45">
         <v>1</v>
       </c>
@@ -9170,9 +9196,9 @@
       <c r="M15" s="45">
         <v>10</v>
       </c>
-      <c r="N15" s="90"/>
-      <c r="R15" s="93"/>
-      <c r="S15" s="93"/>
+      <c r="N15" s="95"/>
+      <c r="R15" s="98"/>
+      <c r="S15" s="98"/>
       <c r="T15" s="45">
         <v>1</v>
       </c>
@@ -9203,9 +9229,9 @@
       <c r="AC15" s="45">
         <v>10</v>
       </c>
-      <c r="AD15" s="90"/>
-      <c r="AG15" s="90"/>
-      <c r="AH15" s="94"/>
+      <c r="AD15" s="95"/>
+      <c r="AG15" s="95"/>
+      <c r="AH15" s="99"/>
       <c r="AI15" s="53" t="s">
         <v>1</v>
       </c>
@@ -9226,7 +9252,7 @@
       </c>
     </row>
     <row r="16" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B16" s="112" t="s">
+      <c r="B16" s="100" t="s">
         <v>110</v>
       </c>
       <c r="C16" s="45" t="s">
@@ -9276,7 +9302,7 @@
         <f>AVERAGE(D16:M16)</f>
         <v>9.5918367346938788E-2</v>
       </c>
-      <c r="R16" s="112" t="s">
+      <c r="R16" s="100" t="s">
         <v>110</v>
       </c>
       <c r="S16" s="45" t="s">
@@ -9322,33 +9348,33 @@
       <c r="AH16" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="AI16" s="111">
+      <c r="AI16" s="59">
         <f>N6</f>
         <v>9.2636986301369864E-2</v>
       </c>
-      <c r="AJ16" s="111">
+      <c r="AJ16" s="59">
         <f>N7</f>
         <v>0.2441780821917808</v>
       </c>
-      <c r="AK16" s="111">
+      <c r="AK16" s="59">
         <f>N8</f>
         <v>0.31849315068493156</v>
       </c>
-      <c r="AL16" s="111">
+      <c r="AL16" s="59">
         <f>N9</f>
         <v>0.49383561643835616</v>
       </c>
-      <c r="AM16" s="111">
+      <c r="AM16" s="59">
         <f>N10</f>
         <v>0.59845890410958913</v>
       </c>
-      <c r="AN16" s="111">
+      <c r="AN16" s="59">
         <f>N11</f>
         <v>0.56746575342465744</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B17" s="112"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="45" t="s">
         <v>2</v>
       </c>
@@ -9396,7 +9422,7 @@
         <f t="shared" ref="N17:N21" si="2">AVERAGE(D17:M17)</f>
         <v>0.19918367346938778</v>
       </c>
-      <c r="R17" s="112"/>
+      <c r="R17" s="100"/>
       <c r="S17" s="45" t="s">
         <v>2</v>
       </c>
@@ -9440,33 +9466,33 @@
       <c r="AH17" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="AI17" s="109">
+      <c r="AI17" s="57">
         <f>N16</f>
         <v>9.5918367346938788E-2</v>
       </c>
-      <c r="AJ17" s="109">
+      <c r="AJ17" s="57">
         <f>N17</f>
         <v>0.19918367346938778</v>
       </c>
-      <c r="AK17" s="109">
+      <c r="AK17" s="57">
         <f>N18</f>
         <v>0.32346938775510203</v>
       </c>
-      <c r="AL17" s="109">
+      <c r="AL17" s="57">
         <f>N19</f>
         <v>0.49091836734693883</v>
       </c>
-      <c r="AM17" s="109">
+      <c r="AM17" s="57">
         <f>N20</f>
         <v>0.54499999999999993</v>
       </c>
-      <c r="AN17" s="109">
+      <c r="AN17" s="57">
         <f>N21</f>
         <v>0.60499999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B18" s="112"/>
+      <c r="B18" s="100"/>
       <c r="C18" s="45" t="s">
         <v>3</v>
       </c>
@@ -9514,7 +9540,7 @@
         <f t="shared" si="2"/>
         <v>0.32346938775510203</v>
       </c>
-      <c r="R18" s="112"/>
+      <c r="R18" s="100"/>
       <c r="S18" s="45" t="s">
         <v>3</v>
       </c>
@@ -9558,23 +9584,23 @@
       <c r="AH18" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="AI18" s="109">
+      <c r="AI18" s="57">
         <f>N26</f>
         <v>0.10015624999999999</v>
       </c>
-      <c r="AJ18" s="109">
+      <c r="AJ18" s="57">
         <f>N27</f>
         <v>0.16820312499999998</v>
       </c>
-      <c r="AK18" s="109">
+      <c r="AK18" s="57">
         <f>N28</f>
         <v>0.37398437499999998</v>
       </c>
-      <c r="AL18" s="109">
+      <c r="AL18" s="57">
         <f>N29</f>
         <v>0.45929687499999999</v>
       </c>
-      <c r="AM18" s="109">
+      <c r="AM18" s="57">
         <f>N30</f>
         <v>0.50226562500000005</v>
       </c>
@@ -9584,7 +9610,7 @@
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B19" s="112"/>
+      <c r="B19" s="100"/>
       <c r="C19" s="45" t="s">
         <v>52</v>
       </c>
@@ -9632,7 +9658,7 @@
         <f t="shared" si="2"/>
         <v>0.49091836734693883</v>
       </c>
-      <c r="R19" s="112"/>
+      <c r="R19" s="100"/>
       <c r="S19" s="45" t="s">
         <v>52</v>
       </c>
@@ -9676,23 +9702,23 @@
       <c r="AH19" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="AI19" s="109">
+      <c r="AI19" s="57">
         <f>N36</f>
         <v>0.10200743494423789</v>
       </c>
-      <c r="AJ19" s="109">
+      <c r="AJ19" s="57">
         <f>N37</f>
         <v>0.16988847583643124</v>
       </c>
-      <c r="AK19" s="109">
+      <c r="AK19" s="57">
         <f>N38</f>
         <v>0.37724907063197022</v>
       </c>
-      <c r="AL19" s="109">
+      <c r="AL19" s="57">
         <f>N39</f>
         <v>0.45933085501858739</v>
       </c>
-      <c r="AM19" s="109">
+      <c r="AM19" s="57">
         <f>N40</f>
         <v>0.54542750929368033</v>
       </c>
@@ -9702,7 +9728,7 @@
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B20" s="112"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="45" t="s">
         <v>51</v>
       </c>
@@ -9750,7 +9776,7 @@
         <f t="shared" si="2"/>
         <v>0.54499999999999993</v>
       </c>
-      <c r="R20" s="112"/>
+      <c r="R20" s="100"/>
       <c r="S20" s="45" t="s">
         <v>51</v>
       </c>
@@ -9790,7 +9816,7 @@
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B21" s="112"/>
+      <c r="B21" s="100"/>
       <c r="C21" s="45" t="s">
         <v>69</v>
       </c>
@@ -9838,7 +9864,7 @@
         <f t="shared" si="2"/>
         <v>0.60499999999999998</v>
       </c>
-      <c r="R21" s="112"/>
+      <c r="R21" s="100"/>
       <c r="S21" s="45" t="s">
         <v>69</v>
       </c>
@@ -9878,48 +9904,48 @@
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B24" s="93" t="s">
+      <c r="B24" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="93"/>
-      <c r="D24" s="94" t="s">
+      <c r="C24" s="98"/>
+      <c r="D24" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="94"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
-      <c r="J24" s="94"/>
-      <c r="K24" s="94"/>
-      <c r="L24" s="94"/>
-      <c r="M24" s="94"/>
-      <c r="N24" s="90" t="s">
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="99"/>
+      <c r="N24" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="R24" s="93" t="s">
+      <c r="R24" s="98" t="s">
         <v>119</v>
       </c>
-      <c r="S24" s="93"/>
-      <c r="T24" s="94" t="s">
+      <c r="S24" s="98"/>
+      <c r="T24" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="U24" s="94"/>
-      <c r="V24" s="94"/>
-      <c r="W24" s="94"/>
-      <c r="X24" s="94"/>
-      <c r="Y24" s="94"/>
-      <c r="Z24" s="94"/>
-      <c r="AA24" s="94"/>
-      <c r="AB24" s="94"/>
-      <c r="AC24" s="94"/>
-      <c r="AD24" s="90" t="s">
+      <c r="U24" s="99"/>
+      <c r="V24" s="99"/>
+      <c r="W24" s="99"/>
+      <c r="X24" s="99"/>
+      <c r="Y24" s="99"/>
+      <c r="Z24" s="99"/>
+      <c r="AA24" s="99"/>
+      <c r="AB24" s="99"/>
+      <c r="AC24" s="99"/>
+      <c r="AD24" s="95" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:40" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="45">
         <v>1</v>
       </c>
@@ -9950,9 +9976,9 @@
       <c r="M25" s="45">
         <v>10</v>
       </c>
-      <c r="N25" s="90"/>
-      <c r="R25" s="93"/>
-      <c r="S25" s="93"/>
+      <c r="N25" s="95"/>
+      <c r="R25" s="98"/>
+      <c r="S25" s="98"/>
       <c r="T25" s="45">
         <v>1</v>
       </c>
@@ -9983,10 +10009,10 @@
       <c r="AC25" s="45">
         <v>10</v>
       </c>
-      <c r="AD25" s="90"/>
+      <c r="AD25" s="95"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B26" s="112" t="s">
+      <c r="B26" s="100" t="s">
         <v>110</v>
       </c>
       <c r="C26" s="45" t="s">
@@ -10036,7 +10062,7 @@
         <f>AVERAGE(D26:M26)</f>
         <v>0.10015624999999999</v>
       </c>
-      <c r="R26" s="112" t="s">
+      <c r="R26" s="100" t="s">
         <v>110</v>
       </c>
       <c r="S26" s="45" t="s">
@@ -10078,7 +10104,7 @@
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B27" s="112"/>
+      <c r="B27" s="100"/>
       <c r="C27" s="45" t="s">
         <v>2</v>
       </c>
@@ -10123,10 +10149,10 @@
         <v>0.28125</v>
       </c>
       <c r="N27" s="50">
-        <f t="shared" ref="N27:N31" si="4">AVERAGE(D27:M27)</f>
+        <f t="shared" ref="N27:N30" si="4">AVERAGE(D27:M27)</f>
         <v>0.16820312499999998</v>
       </c>
-      <c r="R27" s="112"/>
+      <c r="R27" s="100"/>
       <c r="S27" s="45" t="s">
         <v>2</v>
       </c>
@@ -10161,12 +10187,12 @@
         <v>0.104836</v>
       </c>
       <c r="AD27" s="52">
-        <f t="shared" ref="AD27:AD31" si="5">AVERAGE(T27:AC27)</f>
+        <f t="shared" ref="AD27:AD30" si="5">AVERAGE(T27:AC27)</f>
         <v>0.11091480000000001</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B28" s="112"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="45" t="s">
         <v>3</v>
       </c>
@@ -10214,7 +10240,7 @@
         <f t="shared" si="4"/>
         <v>0.37398437499999998</v>
       </c>
-      <c r="R28" s="112"/>
+      <c r="R28" s="100"/>
       <c r="S28" s="45" t="s">
         <v>3</v>
       </c>
@@ -10254,7 +10280,7 @@
       </c>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B29" s="112"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="45" t="s">
         <v>52</v>
       </c>
@@ -10302,7 +10328,7 @@
         <f t="shared" si="4"/>
         <v>0.45929687499999999</v>
       </c>
-      <c r="R29" s="112"/>
+      <c r="R29" s="100"/>
       <c r="S29" s="45" t="s">
         <v>52</v>
       </c>
@@ -10342,7 +10368,7 @@
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B30" s="112"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="45" t="s">
         <v>51</v>
       </c>
@@ -10390,7 +10416,7 @@
         <f t="shared" si="4"/>
         <v>0.50226562500000005</v>
       </c>
-      <c r="R30" s="112"/>
+      <c r="R30" s="100"/>
       <c r="S30" s="45" t="s">
         <v>51</v>
       </c>
@@ -10433,7 +10459,7 @@
       <c r="A31" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="112"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="54" t="s">
         <v>69</v>
       </c>
@@ -10470,7 +10496,7 @@
       <c r="N31" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="R31" s="112"/>
+      <c r="R31" s="100"/>
       <c r="S31" s="54" t="s">
         <v>69</v>
       </c>
@@ -10509,48 +10535,48 @@
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B34" s="93" t="s">
+      <c r="B34" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="93"/>
-      <c r="D34" s="94" t="s">
+      <c r="C34" s="98"/>
+      <c r="D34" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="94"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="94"/>
-      <c r="L34" s="94"/>
-      <c r="M34" s="94"/>
-      <c r="N34" s="90" t="s">
+      <c r="E34" s="99"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
+      <c r="H34" s="99"/>
+      <c r="I34" s="99"/>
+      <c r="J34" s="99"/>
+      <c r="K34" s="99"/>
+      <c r="L34" s="99"/>
+      <c r="M34" s="99"/>
+      <c r="N34" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="R34" s="93" t="s">
+      <c r="R34" s="98" t="s">
         <v>120</v>
       </c>
-      <c r="S34" s="93"/>
-      <c r="T34" s="94" t="s">
+      <c r="S34" s="98"/>
+      <c r="T34" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="U34" s="94"/>
-      <c r="V34" s="94"/>
-      <c r="W34" s="94"/>
-      <c r="X34" s="94"/>
-      <c r="Y34" s="94"/>
-      <c r="Z34" s="94"/>
-      <c r="AA34" s="94"/>
-      <c r="AB34" s="94"/>
-      <c r="AC34" s="94"/>
-      <c r="AD34" s="90" t="s">
+      <c r="U34" s="99"/>
+      <c r="V34" s="99"/>
+      <c r="W34" s="99"/>
+      <c r="X34" s="99"/>
+      <c r="Y34" s="99"/>
+      <c r="Z34" s="99"/>
+      <c r="AA34" s="99"/>
+      <c r="AB34" s="99"/>
+      <c r="AC34" s="99"/>
+      <c r="AD34" s="95" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="93"/>
-      <c r="C35" s="93"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
       <c r="D35" s="45">
         <v>1</v>
       </c>
@@ -10581,9 +10607,9 @@
       <c r="M35" s="45">
         <v>10</v>
       </c>
-      <c r="N35" s="90"/>
-      <c r="R35" s="93"/>
-      <c r="S35" s="93"/>
+      <c r="N35" s="95"/>
+      <c r="R35" s="98"/>
+      <c r="S35" s="98"/>
       <c r="T35" s="45">
         <v>1</v>
       </c>
@@ -10614,10 +10640,10 @@
       <c r="AC35" s="45">
         <v>10</v>
       </c>
-      <c r="AD35" s="90"/>
+      <c r="AD35" s="95"/>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B36" s="112" t="s">
+      <c r="B36" s="100" t="s">
         <v>110</v>
       </c>
       <c r="C36" s="45" t="s">
@@ -10667,7 +10693,7 @@
         <f>AVERAGE(D36:M36)</f>
         <v>0.10200743494423789</v>
       </c>
-      <c r="R36" s="112" t="s">
+      <c r="R36" s="100" t="s">
         <v>110</v>
       </c>
       <c r="S36" s="45" t="s">
@@ -10709,7 +10735,7 @@
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B37" s="112"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="45" t="s">
         <v>2</v>
       </c>
@@ -10754,10 +10780,10 @@
         <v>0.28996282527881045</v>
       </c>
       <c r="N37" s="50">
-        <f t="shared" ref="N37:N41" si="6">AVERAGE(D37:M37)</f>
+        <f t="shared" ref="N37:N40" si="6">AVERAGE(D37:M37)</f>
         <v>0.16988847583643124</v>
       </c>
-      <c r="R37" s="112"/>
+      <c r="R37" s="100"/>
       <c r="S37" s="45" t="s">
         <v>2</v>
       </c>
@@ -10792,12 +10818,12 @@
         <v>0.10981200000000001</v>
       </c>
       <c r="AD37" s="52">
-        <f t="shared" ref="AD37:AD41" si="7">AVERAGE(T37:AC37)</f>
+        <f t="shared" ref="AD37:AD40" si="7">AVERAGE(T37:AC37)</f>
         <v>0.11642079999999999</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B38" s="112"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="45" t="s">
         <v>3</v>
       </c>
@@ -10845,7 +10871,7 @@
         <f t="shared" si="6"/>
         <v>0.37724907063197022</v>
       </c>
-      <c r="R38" s="112"/>
+      <c r="R38" s="100"/>
       <c r="S38" s="45" t="s">
         <v>3</v>
       </c>
@@ -10885,7 +10911,7 @@
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B39" s="112"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="45" t="s">
         <v>52</v>
       </c>
@@ -10933,7 +10959,7 @@
         <f t="shared" si="6"/>
         <v>0.45933085501858739</v>
       </c>
-      <c r="R39" s="112"/>
+      <c r="R39" s="100"/>
       <c r="S39" s="45" t="s">
         <v>52</v>
       </c>
@@ -10973,7 +10999,7 @@
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B40" s="112"/>
+      <c r="B40" s="100"/>
       <c r="C40" s="45" t="s">
         <v>51</v>
       </c>
@@ -11021,7 +11047,7 @@
         <f t="shared" si="6"/>
         <v>0.54542750929368033</v>
       </c>
-      <c r="R40" s="112"/>
+      <c r="R40" s="100"/>
       <c r="S40" s="45" t="s">
         <v>51</v>
       </c>
@@ -11064,7 +11090,7 @@
       <c r="A41" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="112"/>
+      <c r="B41" s="100"/>
       <c r="C41" s="54" t="s">
         <v>69</v>
       </c>
@@ -11101,7 +11127,7 @@
       <c r="N41" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="R41" s="112"/>
+      <c r="R41" s="100"/>
       <c r="S41" s="54" t="s">
         <v>69</v>
       </c>
@@ -11188,7 +11214,1387 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC5CAB5-F7BD-4C9D-9320-5671A06A5F0A}">
+  <dimension ref="B4:X41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="98" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="98"/>
+      <c r="D4" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="S4" s="99" t="s">
+        <v>110</v>
+      </c>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="99"/>
+      <c r="X4" s="99"/>
+    </row>
+    <row r="5" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="56">
+        <v>1</v>
+      </c>
+      <c r="E5" s="56">
+        <v>2</v>
+      </c>
+      <c r="F5" s="56">
+        <v>3</v>
+      </c>
+      <c r="G5" s="56">
+        <v>4</v>
+      </c>
+      <c r="H5" s="56">
+        <v>5</v>
+      </c>
+      <c r="I5" s="56">
+        <v>6</v>
+      </c>
+      <c r="J5" s="56">
+        <v>7</v>
+      </c>
+      <c r="K5" s="56">
+        <v>8</v>
+      </c>
+      <c r="L5" s="56">
+        <v>9</v>
+      </c>
+      <c r="M5" s="56">
+        <v>10</v>
+      </c>
+      <c r="N5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="W5" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" s="60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="51">
+        <v>7.5079999999999999E-3</v>
+      </c>
+      <c r="E6" s="51">
+        <v>2.18E-2</v>
+      </c>
+      <c r="F6" s="51">
+        <v>2.2623999999999998E-2</v>
+      </c>
+      <c r="G6" s="51">
+        <v>2.3324000000000001E-2</v>
+      </c>
+      <c r="H6" s="51">
+        <v>2.2284000000000002E-2</v>
+      </c>
+      <c r="I6" s="51">
+        <v>2.1784000000000001E-2</v>
+      </c>
+      <c r="J6" s="51">
+        <v>2.2352E-2</v>
+      </c>
+      <c r="K6" s="51">
+        <v>2.1624000000000001E-2</v>
+      </c>
+      <c r="L6" s="51">
+        <v>2.1843999999999999E-2</v>
+      </c>
+      <c r="M6" s="51">
+        <v>1.9212E-2</v>
+      </c>
+      <c r="N6" s="52">
+        <f>AVERAGE(D6:M6)</f>
+        <v>2.0435600000000002E-2</v>
+      </c>
+      <c r="Q6" s="60">
+        <v>584</v>
+      </c>
+      <c r="R6" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="S6" s="58">
+        <f>N6</f>
+        <v>2.0435600000000002E-2</v>
+      </c>
+      <c r="T6" s="58">
+        <f>N7</f>
+        <v>1.8062399999999999E-2</v>
+      </c>
+      <c r="U6" s="58">
+        <f>N8</f>
+        <v>1.6647600000000002E-2</v>
+      </c>
+      <c r="V6" s="58">
+        <f>N9</f>
+        <v>1.3285999999999997E-2</v>
+      </c>
+      <c r="W6" s="58">
+        <f>N10</f>
+        <v>1.1668800000000002E-2</v>
+      </c>
+      <c r="X6" s="58">
+        <f>N11</f>
+        <v>1.1855599999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="100"/>
+      <c r="C7" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="51">
+        <v>4.9399999999999999E-3</v>
+      </c>
+      <c r="E7" s="51">
+        <v>2.1284000000000001E-2</v>
+      </c>
+      <c r="F7" s="51">
+        <v>2.0587999999999999E-2</v>
+      </c>
+      <c r="G7" s="51">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="H7" s="51">
+        <v>2.1548000000000001E-2</v>
+      </c>
+      <c r="I7" s="51">
+        <v>1.8475999999999999E-2</v>
+      </c>
+      <c r="J7" s="51">
+        <v>2.0104E-2</v>
+      </c>
+      <c r="K7" s="51">
+        <v>1.2319999999999999E-2</v>
+      </c>
+      <c r="L7" s="51">
+        <v>2.1484E-2</v>
+      </c>
+      <c r="M7" s="51">
+        <v>1.728E-2</v>
+      </c>
+      <c r="N7" s="52">
+        <f t="shared" ref="N7:N11" si="0">AVERAGE(D7:M7)</f>
+        <v>1.8062399999999999E-2</v>
+      </c>
+      <c r="Q7" s="60">
+        <v>980</v>
+      </c>
+      <c r="R7" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="S7" s="43">
+        <f>N16</f>
+        <v>3.3833199999999994E-2</v>
+      </c>
+      <c r="T7" s="43">
+        <f>N17</f>
+        <v>3.1182000000000005E-2</v>
+      </c>
+      <c r="U7" s="43">
+        <f>N18</f>
+        <v>2.74644E-2</v>
+      </c>
+      <c r="V7" s="43">
+        <f>N19</f>
+        <v>2.2094399999999997E-2</v>
+      </c>
+      <c r="W7" s="43">
+        <f>N20</f>
+        <v>1.983E-2</v>
+      </c>
+      <c r="X7" s="43">
+        <f>N21</f>
+        <v>1.8287599999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="100"/>
+      <c r="C8" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="51">
+        <v>4.0280000000000003E-3</v>
+      </c>
+      <c r="E8" s="51">
+        <v>2.0812000000000001E-2</v>
+      </c>
+      <c r="F8" s="51">
+        <v>1.8168E-2</v>
+      </c>
+      <c r="G8" s="51">
+        <v>2.1635999999999999E-2</v>
+      </c>
+      <c r="H8" s="51">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="I8" s="51">
+        <v>1.5712E-2</v>
+      </c>
+      <c r="J8" s="51">
+        <v>2.034E-2</v>
+      </c>
+      <c r="K8" s="51">
+        <v>8.4200000000000004E-3</v>
+      </c>
+      <c r="L8" s="51">
+        <v>2.0184000000000001E-2</v>
+      </c>
+      <c r="M8" s="51">
+        <v>1.5476E-2</v>
+      </c>
+      <c r="N8" s="52">
+        <f t="shared" si="0"/>
+        <v>1.6647600000000002E-2</v>
+      </c>
+      <c r="Q8" s="60">
+        <v>1280</v>
+      </c>
+      <c r="R8" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="S8" s="43">
+        <f>N26</f>
+        <v>4.4414799999999997E-2</v>
+      </c>
+      <c r="T8" s="43">
+        <f>N27</f>
+        <v>4.2452000000000004E-2</v>
+      </c>
+      <c r="U8" s="43">
+        <f>N28</f>
+        <v>3.4628800000000001E-2</v>
+      </c>
+      <c r="V8" s="43">
+        <f>N29</f>
+        <v>3.0598800000000002E-2</v>
+      </c>
+      <c r="W8" s="43">
+        <f>N30</f>
+        <v>2.77308E-2</v>
+      </c>
+      <c r="X8" s="54" t="str">
+        <f>N31</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" s="100"/>
+      <c r="C9" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="51">
+        <v>3.5560000000000001E-3</v>
+      </c>
+      <c r="E9" s="51">
+        <v>2.1135999999999999E-2</v>
+      </c>
+      <c r="F9" s="51">
+        <v>1.7323999999999999E-2</v>
+      </c>
+      <c r="G9" s="51">
+        <v>2.1243999999999999E-2</v>
+      </c>
+      <c r="H9" s="51">
+        <v>2.0619999999999999E-2</v>
+      </c>
+      <c r="I9" s="51">
+        <v>7.9719999999999999E-3</v>
+      </c>
+      <c r="J9" s="51">
+        <v>9.9120000000000007E-3</v>
+      </c>
+      <c r="K9" s="51">
+        <v>7.3920000000000001E-3</v>
+      </c>
+      <c r="L9" s="51">
+        <v>8.7279999999999996E-3</v>
+      </c>
+      <c r="M9" s="51">
+        <v>1.4976E-2</v>
+      </c>
+      <c r="N9" s="52">
+        <f t="shared" si="0"/>
+        <v>1.3285999999999997E-2</v>
+      </c>
+      <c r="Q9" s="60">
+        <v>1345</v>
+      </c>
+      <c r="R9" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="S9" s="43">
+        <f>N36</f>
+        <v>4.6591200000000006E-2</v>
+      </c>
+      <c r="T9" s="43">
+        <f>N37</f>
+        <v>4.45184E-2</v>
+      </c>
+      <c r="U9" s="43">
+        <f>N38</f>
+        <v>3.6243600000000001E-2</v>
+      </c>
+      <c r="V9" s="43">
+        <f>N39</f>
+        <v>3.2141200000000002E-2</v>
+      </c>
+      <c r="W9" s="43">
+        <f>N40</f>
+        <v>2.8977599999999999E-2</v>
+      </c>
+      <c r="X9" s="54" t="str">
+        <f>N41</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="100"/>
+      <c r="C10" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="51">
+        <v>3.3159999999999999E-3</v>
+      </c>
+      <c r="E10" s="51">
+        <v>1.7804E-2</v>
+      </c>
+      <c r="F10" s="51">
+        <v>1.7347999999999999E-2</v>
+      </c>
+      <c r="G10" s="51">
+        <v>1.3976000000000001E-2</v>
+      </c>
+      <c r="H10" s="51">
+        <v>1.5072E-2</v>
+      </c>
+      <c r="I10" s="51">
+        <v>8.064E-3</v>
+      </c>
+      <c r="J10" s="51">
+        <v>9.8600000000000007E-3</v>
+      </c>
+      <c r="K10" s="51">
+        <v>7.456E-3</v>
+      </c>
+      <c r="L10" s="51">
+        <v>8.8800000000000007E-3</v>
+      </c>
+      <c r="M10" s="51">
+        <v>1.4912E-2</v>
+      </c>
+      <c r="N10" s="52">
+        <f t="shared" si="0"/>
+        <v>1.1668800000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" s="100"/>
+      <c r="C11" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="51">
+        <v>3.2520000000000001E-3</v>
+      </c>
+      <c r="E11" s="51">
+        <v>1.7548000000000001E-2</v>
+      </c>
+      <c r="F11" s="51">
+        <v>1.7663999999999999E-2</v>
+      </c>
+      <c r="G11" s="51">
+        <v>1.4423999999999999E-2</v>
+      </c>
+      <c r="H11" s="51">
+        <v>1.4683999999999999E-2</v>
+      </c>
+      <c r="I11" s="51">
+        <v>8.3320000000000009E-3</v>
+      </c>
+      <c r="J11" s="51">
+        <v>1.0196E-2</v>
+      </c>
+      <c r="K11" s="51">
+        <v>7.7679999999999997E-3</v>
+      </c>
+      <c r="L11" s="51">
+        <v>9.2239999999999996E-3</v>
+      </c>
+      <c r="M11" s="51">
+        <v>1.5464E-2</v>
+      </c>
+      <c r="N11" s="52">
+        <f t="shared" si="0"/>
+        <v>1.1855599999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="98" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="98"/>
+      <c r="D14" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="95" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="56">
+        <v>1</v>
+      </c>
+      <c r="E15" s="56">
+        <v>2</v>
+      </c>
+      <c r="F15" s="56">
+        <v>3</v>
+      </c>
+      <c r="G15" s="56">
+        <v>4</v>
+      </c>
+      <c r="H15" s="56">
+        <v>5</v>
+      </c>
+      <c r="I15" s="56">
+        <v>6</v>
+      </c>
+      <c r="J15" s="56">
+        <v>7</v>
+      </c>
+      <c r="K15" s="56">
+        <v>8</v>
+      </c>
+      <c r="L15" s="56">
+        <v>9</v>
+      </c>
+      <c r="M15" s="56">
+        <v>10</v>
+      </c>
+      <c r="N15" s="95"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="51">
+        <v>1.2284E-2</v>
+      </c>
+      <c r="E16" s="51">
+        <v>3.5875999999999998E-2</v>
+      </c>
+      <c r="F16" s="51">
+        <v>3.5027999999999997E-2</v>
+      </c>
+      <c r="G16" s="51">
+        <v>3.6415999999999997E-2</v>
+      </c>
+      <c r="H16" s="51">
+        <v>3.6991999999999997E-2</v>
+      </c>
+      <c r="I16" s="51">
+        <v>3.6704000000000001E-2</v>
+      </c>
+      <c r="J16" s="51">
+        <v>3.3568000000000001E-2</v>
+      </c>
+      <c r="K16" s="51">
+        <v>3.7859999999999998E-2</v>
+      </c>
+      <c r="L16" s="51">
+        <v>3.6616000000000003E-2</v>
+      </c>
+      <c r="M16" s="51">
+        <v>3.6988E-2</v>
+      </c>
+      <c r="N16" s="52">
+        <f>AVERAGE(D16:M16)</f>
+        <v>3.3833199999999994E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="100"/>
+      <c r="C17" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="51">
+        <v>9.1319999999999995E-3</v>
+      </c>
+      <c r="E17" s="51">
+        <v>3.5380000000000002E-2</v>
+      </c>
+      <c r="F17" s="51">
+        <v>3.3959999999999997E-2</v>
+      </c>
+      <c r="G17" s="51">
+        <v>3.058E-2</v>
+      </c>
+      <c r="H17" s="51">
+        <v>3.3015999999999997E-2</v>
+      </c>
+      <c r="I17" s="51">
+        <v>3.1452000000000001E-2</v>
+      </c>
+      <c r="J17" s="51">
+        <v>3.3584000000000003E-2</v>
+      </c>
+      <c r="K17" s="51">
+        <v>3.7476000000000002E-2</v>
+      </c>
+      <c r="L17" s="51">
+        <v>3.3700000000000001E-2</v>
+      </c>
+      <c r="M17" s="51">
+        <v>3.354E-2</v>
+      </c>
+      <c r="N17" s="52">
+        <f t="shared" ref="N17:N21" si="1">AVERAGE(D17:M17)</f>
+        <v>3.1182000000000005E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="100"/>
+      <c r="C18" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="51">
+        <v>6.3359999999999996E-3</v>
+      </c>
+      <c r="E18" s="51">
+        <v>3.5096000000000002E-2</v>
+      </c>
+      <c r="F18" s="51">
+        <v>3.1668000000000002E-2</v>
+      </c>
+      <c r="G18" s="51">
+        <v>2.5748E-2</v>
+      </c>
+      <c r="H18" s="51">
+        <v>3.1815999999999997E-2</v>
+      </c>
+      <c r="I18" s="51">
+        <v>2.2259999999999999E-2</v>
+      </c>
+      <c r="J18" s="51">
+        <v>3.4020000000000002E-2</v>
+      </c>
+      <c r="K18" s="51">
+        <v>2.9592E-2</v>
+      </c>
+      <c r="L18" s="51">
+        <v>2.9059999999999999E-2</v>
+      </c>
+      <c r="M18" s="51">
+        <v>2.9048000000000001E-2</v>
+      </c>
+      <c r="N18" s="52">
+        <f t="shared" si="1"/>
+        <v>2.74644E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="100"/>
+      <c r="C19" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="51">
+        <v>5.5240000000000003E-3</v>
+      </c>
+      <c r="E19" s="51">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="F19" s="51">
+        <v>2.8087999999999998E-2</v>
+      </c>
+      <c r="G19" s="51">
+        <v>1.3847999999999999E-2</v>
+      </c>
+      <c r="H19" s="51">
+        <v>3.1940000000000003E-2</v>
+      </c>
+      <c r="I19" s="51">
+        <v>1.4696000000000001E-2</v>
+      </c>
+      <c r="J19" s="51">
+        <v>1.5896E-2</v>
+      </c>
+      <c r="K19" s="51">
+        <v>2.222E-2</v>
+      </c>
+      <c r="L19" s="51">
+        <v>2.6915999999999999E-2</v>
+      </c>
+      <c r="M19" s="51">
+        <v>2.6315999999999999E-2</v>
+      </c>
+      <c r="N19" s="52">
+        <f t="shared" si="1"/>
+        <v>2.2094399999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="100"/>
+      <c r="C20" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="51">
+        <v>5.1120000000000002E-3</v>
+      </c>
+      <c r="E20" s="51">
+        <v>2.4004000000000001E-2</v>
+      </c>
+      <c r="F20" s="51">
+        <v>2.4576000000000001E-2</v>
+      </c>
+      <c r="G20" s="51">
+        <v>1.4083999999999999E-2</v>
+      </c>
+      <c r="H20" s="51">
+        <v>2.8384E-2</v>
+      </c>
+      <c r="I20" s="51">
+        <v>1.2812E-2</v>
+      </c>
+      <c r="J20" s="51">
+        <v>1.5587999999999999E-2</v>
+      </c>
+      <c r="K20" s="51">
+        <v>2.2248E-2</v>
+      </c>
+      <c r="L20" s="51">
+        <v>2.5992000000000001E-2</v>
+      </c>
+      <c r="M20" s="51">
+        <v>2.5499999999999998E-2</v>
+      </c>
+      <c r="N20" s="52">
+        <f t="shared" si="1"/>
+        <v>1.983E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="100"/>
+      <c r="C21" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="51">
+        <v>4.9800000000000001E-3</v>
+      </c>
+      <c r="E21" s="51">
+        <v>2.3647999999999999E-2</v>
+      </c>
+      <c r="F21" s="51">
+        <v>2.3448E-2</v>
+      </c>
+      <c r="G21" s="51">
+        <v>1.4484E-2</v>
+      </c>
+      <c r="H21" s="51">
+        <v>1.7083999999999998E-2</v>
+      </c>
+      <c r="I21" s="51">
+        <v>9.5040000000000003E-3</v>
+      </c>
+      <c r="J21" s="51">
+        <v>1.5827999999999998E-2</v>
+      </c>
+      <c r="K21" s="51">
+        <v>2.2508E-2</v>
+      </c>
+      <c r="L21" s="51">
+        <v>2.5995999999999998E-2</v>
+      </c>
+      <c r="M21" s="51">
+        <v>2.5395999999999998E-2</v>
+      </c>
+      <c r="N21" s="52">
+        <f t="shared" si="1"/>
+        <v>1.8287599999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="98"/>
+      <c r="D24" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="99"/>
+      <c r="N24" s="95" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="98"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="56">
+        <v>1</v>
+      </c>
+      <c r="E25" s="56">
+        <v>2</v>
+      </c>
+      <c r="F25" s="56">
+        <v>3</v>
+      </c>
+      <c r="G25" s="56">
+        <v>4</v>
+      </c>
+      <c r="H25" s="56">
+        <v>5</v>
+      </c>
+      <c r="I25" s="56">
+        <v>6</v>
+      </c>
+      <c r="J25" s="56">
+        <v>7</v>
+      </c>
+      <c r="K25" s="56">
+        <v>8</v>
+      </c>
+      <c r="L25" s="56">
+        <v>9</v>
+      </c>
+      <c r="M25" s="56">
+        <v>10</v>
+      </c>
+      <c r="N25" s="95"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="51">
+        <v>1.5876000000000001E-2</v>
+      </c>
+      <c r="E26" s="51">
+        <v>4.6615999999999998E-2</v>
+      </c>
+      <c r="F26" s="51">
+        <v>4.9723999999999997E-2</v>
+      </c>
+      <c r="G26" s="51">
+        <v>4.7216000000000001E-2</v>
+      </c>
+      <c r="H26" s="51">
+        <v>4.9571999999999998E-2</v>
+      </c>
+      <c r="I26" s="51">
+        <v>4.9604000000000002E-2</v>
+      </c>
+      <c r="J26" s="51">
+        <v>4.4403999999999999E-2</v>
+      </c>
+      <c r="K26" s="51">
+        <v>4.9548000000000002E-2</v>
+      </c>
+      <c r="L26" s="51">
+        <v>4.9647999999999998E-2</v>
+      </c>
+      <c r="M26" s="51">
+        <v>4.1939999999999998E-2</v>
+      </c>
+      <c r="N26" s="52">
+        <f>AVERAGE(D26:M26)</f>
+        <v>4.4414799999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="100"/>
+      <c r="C27" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="51">
+        <v>1.1808000000000001E-2</v>
+      </c>
+      <c r="E27" s="51">
+        <v>4.6156000000000003E-2</v>
+      </c>
+      <c r="F27" s="51">
+        <v>4.9404000000000003E-2</v>
+      </c>
+      <c r="G27" s="51">
+        <v>4.054E-2</v>
+      </c>
+      <c r="H27" s="51">
+        <v>4.8236000000000001E-2</v>
+      </c>
+      <c r="I27" s="51">
+        <v>4.8076000000000001E-2</v>
+      </c>
+      <c r="J27" s="51">
+        <v>4.2816E-2</v>
+      </c>
+      <c r="K27" s="51">
+        <v>4.8660000000000002E-2</v>
+      </c>
+      <c r="L27" s="51">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="M27" s="51">
+        <v>3.9523999999999997E-2</v>
+      </c>
+      <c r="N27" s="52">
+        <f t="shared" ref="N27:N30" si="2">AVERAGE(D27:M27)</f>
+        <v>4.2452000000000004E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="100"/>
+      <c r="C28" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="51">
+        <v>9.5440000000000004E-3</v>
+      </c>
+      <c r="E28" s="51">
+        <v>4.6019999999999998E-2</v>
+      </c>
+      <c r="F28" s="51">
+        <v>4.2028000000000003E-2</v>
+      </c>
+      <c r="G28" s="51">
+        <v>3.7892000000000002E-2</v>
+      </c>
+      <c r="H28" s="51">
+        <v>4.5032000000000003E-2</v>
+      </c>
+      <c r="I28" s="51">
+        <v>3.9488000000000002E-2</v>
+      </c>
+      <c r="J28" s="51">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="K28" s="51">
+        <v>2.3619999999999999E-2</v>
+      </c>
+      <c r="L28" s="51">
+        <v>2.2651999999999999E-2</v>
+      </c>
+      <c r="M28" s="51">
+        <v>3.8011999999999997E-2</v>
+      </c>
+      <c r="N28" s="52">
+        <f t="shared" si="2"/>
+        <v>3.4628800000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="100"/>
+      <c r="C29" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="51">
+        <v>7.0239999999999999E-3</v>
+      </c>
+      <c r="E29" s="51">
+        <v>4.4915999999999998E-2</v>
+      </c>
+      <c r="F29" s="51">
+        <v>3.1671999999999999E-2</v>
+      </c>
+      <c r="G29" s="51">
+        <v>3.2804E-2</v>
+      </c>
+      <c r="H29" s="51">
+        <v>4.1579999999999999E-2</v>
+      </c>
+      <c r="I29" s="51">
+        <v>3.9620000000000002E-2</v>
+      </c>
+      <c r="J29" s="51">
+        <v>4.1588E-2</v>
+      </c>
+      <c r="K29" s="51">
+        <v>1.5384E-2</v>
+      </c>
+      <c r="L29" s="51">
+        <v>1.536E-2</v>
+      </c>
+      <c r="M29" s="51">
+        <v>3.6040000000000003E-2</v>
+      </c>
+      <c r="N29" s="52">
+        <f t="shared" si="2"/>
+        <v>3.0598800000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="100"/>
+      <c r="C30" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="51">
+        <v>6.4879999999999998E-3</v>
+      </c>
+      <c r="E30" s="51">
+        <v>2.5947999999999999E-2</v>
+      </c>
+      <c r="F30" s="51">
+        <v>2.9416000000000001E-2</v>
+      </c>
+      <c r="G30" s="51">
+        <v>3.1859999999999999E-2</v>
+      </c>
+      <c r="H30" s="51">
+        <v>3.9239999999999997E-2</v>
+      </c>
+      <c r="I30" s="51">
+        <v>3.7412000000000001E-2</v>
+      </c>
+      <c r="J30" s="51">
+        <v>4.0564000000000003E-2</v>
+      </c>
+      <c r="K30" s="51">
+        <v>1.5192000000000001E-2</v>
+      </c>
+      <c r="L30" s="51">
+        <v>1.5192000000000001E-2</v>
+      </c>
+      <c r="M30" s="51">
+        <v>3.5996E-2</v>
+      </c>
+      <c r="N30" s="52">
+        <f t="shared" si="2"/>
+        <v>2.77308E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="100"/>
+      <c r="C31" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="K31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="L31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="M31" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="N31" s="55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="98" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="98"/>
+      <c r="D34" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="99"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
+      <c r="H34" s="99"/>
+      <c r="I34" s="99"/>
+      <c r="J34" s="99"/>
+      <c r="K34" s="99"/>
+      <c r="L34" s="99"/>
+      <c r="M34" s="99"/>
+      <c r="N34" s="95" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="56">
+        <v>1</v>
+      </c>
+      <c r="E35" s="56">
+        <v>2</v>
+      </c>
+      <c r="F35" s="56">
+        <v>3</v>
+      </c>
+      <c r="G35" s="56">
+        <v>4</v>
+      </c>
+      <c r="H35" s="56">
+        <v>5</v>
+      </c>
+      <c r="I35" s="56">
+        <v>6</v>
+      </c>
+      <c r="J35" s="56">
+        <v>7</v>
+      </c>
+      <c r="K35" s="56">
+        <v>8</v>
+      </c>
+      <c r="L35" s="56">
+        <v>9</v>
+      </c>
+      <c r="M35" s="56">
+        <v>10</v>
+      </c>
+      <c r="N35" s="95"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="51">
+        <v>1.6643999999999999E-2</v>
+      </c>
+      <c r="E36" s="51">
+        <v>4.8787999999999998E-2</v>
+      </c>
+      <c r="F36" s="51">
+        <v>5.2207999999999997E-2</v>
+      </c>
+      <c r="G36" s="51">
+        <v>4.9627999999999999E-2</v>
+      </c>
+      <c r="H36" s="51">
+        <v>5.1996000000000001E-2</v>
+      </c>
+      <c r="I36" s="51">
+        <v>5.1872000000000001E-2</v>
+      </c>
+      <c r="J36" s="51">
+        <v>4.6696000000000001E-2</v>
+      </c>
+      <c r="K36" s="51">
+        <v>5.2012000000000003E-2</v>
+      </c>
+      <c r="L36" s="51">
+        <v>5.2156000000000001E-2</v>
+      </c>
+      <c r="M36" s="51">
+        <v>4.3912E-2</v>
+      </c>
+      <c r="N36" s="52">
+        <f>AVERAGE(D36:M36)</f>
+        <v>4.6591200000000006E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="100"/>
+      <c r="C37" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="51">
+        <v>1.2376E-2</v>
+      </c>
+      <c r="E37" s="51">
+        <v>4.8379999999999999E-2</v>
+      </c>
+      <c r="F37" s="51">
+        <v>5.1903999999999999E-2</v>
+      </c>
+      <c r="G37" s="51">
+        <v>4.2403999999999997E-2</v>
+      </c>
+      <c r="H37" s="51">
+        <v>5.0687999999999997E-2</v>
+      </c>
+      <c r="I37" s="51">
+        <v>5.0104000000000003E-2</v>
+      </c>
+      <c r="J37" s="51">
+        <v>4.5143999999999997E-2</v>
+      </c>
+      <c r="K37" s="51">
+        <v>5.1128E-2</v>
+      </c>
+      <c r="L37" s="51">
+        <v>5.1796000000000002E-2</v>
+      </c>
+      <c r="M37" s="51">
+        <v>4.1259999999999998E-2</v>
+      </c>
+      <c r="N37" s="52">
+        <f t="shared" ref="N37:N40" si="3">AVERAGE(D37:M37)</f>
+        <v>4.45184E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="100"/>
+      <c r="C38" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="51">
+        <v>1.0012E-2</v>
+      </c>
+      <c r="E38" s="51">
+        <v>4.8287999999999998E-2</v>
+      </c>
+      <c r="F38" s="51">
+        <v>4.3344000000000001E-2</v>
+      </c>
+      <c r="G38" s="51">
+        <v>3.9416E-2</v>
+      </c>
+      <c r="H38" s="51">
+        <v>4.7287999999999997E-2</v>
+      </c>
+      <c r="I38" s="51">
+        <v>4.1604000000000002E-2</v>
+      </c>
+      <c r="J38" s="51">
+        <v>4.4268000000000002E-2</v>
+      </c>
+      <c r="K38" s="51">
+        <v>2.4572E-2</v>
+      </c>
+      <c r="L38" s="51">
+        <v>2.384E-2</v>
+      </c>
+      <c r="M38" s="51">
+        <v>3.9803999999999999E-2</v>
+      </c>
+      <c r="N38" s="52">
+        <f t="shared" si="3"/>
+        <v>3.6243600000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="100"/>
+      <c r="C39" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="51">
+        <v>7.3359999999999996E-3</v>
+      </c>
+      <c r="E39" s="51">
+        <v>4.7224000000000002E-2</v>
+      </c>
+      <c r="F39" s="51">
+        <v>3.3020000000000001E-2</v>
+      </c>
+      <c r="G39" s="51">
+        <v>3.4320000000000003E-2</v>
+      </c>
+      <c r="H39" s="51">
+        <v>4.3647999999999999E-2</v>
+      </c>
+      <c r="I39" s="51">
+        <v>4.1716000000000003E-2</v>
+      </c>
+      <c r="J39" s="51">
+        <v>4.3864E-2</v>
+      </c>
+      <c r="K39" s="51">
+        <v>1.6112000000000001E-2</v>
+      </c>
+      <c r="L39" s="51">
+        <v>1.6448000000000001E-2</v>
+      </c>
+      <c r="M39" s="51">
+        <v>3.7724000000000001E-2</v>
+      </c>
+      <c r="N39" s="52">
+        <f t="shared" si="3"/>
+        <v>3.2141200000000002E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="100"/>
+      <c r="C40" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="51">
+        <v>6.816E-3</v>
+      </c>
+      <c r="E40" s="51">
+        <v>2.6388000000000002E-2</v>
+      </c>
+      <c r="F40" s="51">
+        <v>3.0504E-2</v>
+      </c>
+      <c r="G40" s="51">
+        <v>3.3304E-2</v>
+      </c>
+      <c r="H40" s="51">
+        <v>4.1251999999999997E-2</v>
+      </c>
+      <c r="I40" s="51">
+        <v>3.9376000000000001E-2</v>
+      </c>
+      <c r="J40" s="51">
+        <v>4.2684E-2</v>
+      </c>
+      <c r="K40" s="51">
+        <v>1.5911999999999999E-2</v>
+      </c>
+      <c r="L40" s="51">
+        <v>1.5807999999999999E-2</v>
+      </c>
+      <c r="M40" s="51">
+        <v>3.7732000000000002E-2</v>
+      </c>
+      <c r="N40" s="52">
+        <f>AVERAGE(D40:M40)</f>
+        <v>2.8977599999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="100"/>
+      <c r="C41" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="I41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="J41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="K41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="L41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="M41" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="N41" s="55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:X4"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:M4"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:M14"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:M24"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:M34"/>
+    <mergeCell ref="N34:N35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B6:R38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11262,7 +12668,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="97">
+      <c r="B8" s="103">
         <v>584</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -11283,7 +12689,7 @@
       <c r="H8" s="1">
         <v>8.0800000000000004E-3</v>
       </c>
-      <c r="L8" s="98">
+      <c r="L8" s="104">
         <v>584</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -11306,7 +12712,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="97"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="1" t="s">
         <v>68</v>
       </c>
@@ -11325,7 +12731,7 @@
       <c r="H9" s="1">
         <v>4.5935999999999998E-2</v>
       </c>
-      <c r="L9" s="99"/>
+      <c r="L9" s="105"/>
       <c r="M9" s="1" t="s">
         <v>65</v>
       </c>
@@ -11351,7 +12757,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="95">
+      <c r="B10" s="101">
         <v>980</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -11372,7 +12778,7 @@
       <c r="H10" s="16">
         <v>1.2456E-2</v>
       </c>
-      <c r="L10" s="99"/>
+      <c r="L10" s="105"/>
       <c r="M10" s="1" t="s">
         <v>61</v>
       </c>
@@ -11393,7 +12799,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="95"/>
+      <c r="B11" s="101"/>
       <c r="C11" s="16" t="s">
         <v>68</v>
       </c>
@@ -11412,7 +12818,7 @@
       <c r="H11" s="16">
         <v>6.3119999999999996E-2</v>
       </c>
-      <c r="L11" s="100"/>
+      <c r="L11" s="106"/>
       <c r="M11" s="1" t="s">
         <v>66</v>
       </c>
@@ -11438,7 +12844,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="94">
+      <c r="B12" s="99">
         <v>1280</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -11459,7 +12865,7 @@
       <c r="H12" s="4">
         <v>1.5299999999999999E-2</v>
       </c>
-      <c r="L12" s="101">
+      <c r="L12" s="107">
         <v>980</v>
       </c>
       <c r="M12" s="16" t="s">
@@ -11482,7 +12888,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="94"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="4" t="s">
         <v>68</v>
       </c>
@@ -11501,7 +12907,7 @@
       <c r="H13" s="4">
         <v>6.6844000000000001E-2</v>
       </c>
-      <c r="L13" s="102"/>
+      <c r="L13" s="108"/>
       <c r="M13" s="16" t="s">
         <v>66</v>
       </c>
@@ -11527,7 +12933,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="96">
+      <c r="B14" s="102">
         <v>1345</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -11548,7 +12954,7 @@
       <c r="H14" s="7">
         <v>1.5807999999999999E-2</v>
       </c>
-      <c r="L14" s="102"/>
+      <c r="L14" s="108"/>
       <c r="M14" s="16" t="s">
         <v>61</v>
       </c>
@@ -11569,7 +12975,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="96"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="7" t="s">
         <v>68</v>
       </c>
@@ -11588,7 +12994,7 @@
       <c r="H15" s="7">
         <v>6.7227999999999996E-2</v>
       </c>
-      <c r="L15" s="103"/>
+      <c r="L15" s="109"/>
       <c r="M15" s="16" t="s">
         <v>66</v>
       </c>
@@ -11614,7 +13020,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L16" s="104">
+      <c r="L16" s="110">
         <v>1280</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -11637,7 +13043,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L17" s="105"/>
+      <c r="L17" s="111"/>
       <c r="M17" s="4" t="s">
         <v>65</v>
       </c>
@@ -11663,7 +13069,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L18" s="105"/>
+      <c r="L18" s="111"/>
       <c r="M18" s="4" t="s">
         <v>61</v>
       </c>
@@ -11684,7 +13090,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L19" s="106"/>
+      <c r="L19" s="112"/>
       <c r="M19" s="4" t="s">
         <v>65</v>
       </c>
@@ -11710,7 +13116,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L20" s="96">
+      <c r="L20" s="102">
         <v>1345</v>
       </c>
       <c r="M20" s="7" t="s">
@@ -11733,7 +13139,7 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L21" s="96"/>
+      <c r="L21" s="102"/>
       <c r="M21" s="7" t="s">
         <v>65</v>
       </c>
@@ -11759,7 +13165,7 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L22" s="96"/>
+      <c r="L22" s="102"/>
       <c r="M22" s="7" t="s">
         <v>61</v>
       </c>
@@ -11780,7 +13186,7 @@
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L23" s="96"/>
+      <c r="L23" s="102"/>
       <c r="M23" s="7" t="s">
         <v>65</v>
       </c>
@@ -11834,7 +13240,7 @@
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="97">
+      <c r="B31" s="103">
         <v>584</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -11857,7 +13263,7 @@
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="97"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="1" t="s">
         <v>68</v>
       </c>
@@ -11878,7 +13284,7 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="95">
+      <c r="B33" s="101">
         <v>980</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -11901,7 +13307,7 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="95"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="16" t="s">
         <v>68</v>
       </c>
@@ -11922,7 +13328,7 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="94">
+      <c r="B35" s="99">
         <v>1280</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -11945,7 +13351,7 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="94"/>
+      <c r="B36" s="99"/>
       <c r="C36" s="4" t="s">
         <v>68</v>
       </c>
@@ -11966,7 +13372,7 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="96">
+      <c r="B37" s="102">
         <v>1345</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -11989,7 +13395,7 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="96"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="7" t="s">
         <v>68</v>
       </c>
@@ -12029,8 +13435,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A5:R19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -12048,7 +13454,7 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="113" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -12074,7 +13480,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
+      <c r="A6" s="113"/>
       <c r="B6" s="33">
         <v>584</v>
       </c>
@@ -12098,7 +13504,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
+      <c r="A7" s="113"/>
       <c r="B7" s="33">
         <v>980</v>
       </c>
@@ -12122,7 +13528,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
+      <c r="A8" s="113"/>
       <c r="B8" s="33">
         <v>1280</v>
       </c>
@@ -12146,7 +13552,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="33">
         <v>1435</v>
       </c>
@@ -12170,7 +13576,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="33">
         <v>1640</v>
       </c>
@@ -12194,7 +13600,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="107" t="s">
+      <c r="A14" s="113" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -12220,7 +13626,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
+      <c r="A15" s="113"/>
       <c r="B15" s="33">
         <v>584</v>
       </c>
@@ -12232,7 +13638,7 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+      <c r="A16" s="113"/>
       <c r="B16" s="33">
         <v>980</v>
       </c>
@@ -12242,11 +13648,11 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="5"/>
-      <c r="K16" s="108" t="s">
+      <c r="K16" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="108"/>
-      <c r="M16" s="108"/>
+      <c r="L16" s="114"/>
+      <c r="M16" s="114"/>
       <c r="P16" s="11" t="s">
         <v>80</v>
       </c>
@@ -12258,7 +13664,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+      <c r="A17" s="113"/>
       <c r="B17" s="33">
         <v>1280</v>
       </c>
@@ -12288,7 +13694,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="107"/>
+      <c r="A18" s="113"/>
       <c r="B18" s="33">
         <v>1435</v>
       </c>
@@ -12318,7 +13724,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
+      <c r="A19" s="113"/>
       <c r="B19" s="33">
         <v>1640</v>
       </c>

</xml_diff>